<commit_message>
Added up to 50
</commit_message>
<xml_diff>
--- a/accident_ground_truths.xlsx
+++ b/accident_ground_truths.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E206E37-094D-4013-BEBD-90D417093475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5671703E-7049-4032-A39B-6F10C41755ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="141">
   <si>
     <t>Number of vehicles in accident</t>
   </si>
@@ -158,6 +158,291 @@
   </si>
   <si>
     <t>Truck lightly taps suv and enters median. This could possibly lead to other impacts with oncoming traffic</t>
+  </si>
+  <si>
+    <t>sedan x2</t>
+  </si>
+  <si>
+    <t>Night, hard to see</t>
+  </si>
+  <si>
+    <t>One sedan was a taxi, happened at a traffic light</t>
+  </si>
+  <si>
+    <t>side-on-side collision</t>
+  </si>
+  <si>
+    <t>Looks to be a busy intersection, and does not look like too serious a collision compared to most accidents</t>
+  </si>
+  <si>
+    <t>front-to-front-side collision</t>
+  </si>
+  <si>
+    <t>Day, cloudy, possible rain?</t>
+  </si>
+  <si>
+    <t>One sedan caused the other to spin out a little, debris was shown</t>
+  </si>
+  <si>
+    <t>Day, cloudy</t>
+  </si>
+  <si>
+    <t>Sedan ran a red light</t>
+  </si>
+  <si>
+    <t>One sedan ran a red light and got hit</t>
+  </si>
+  <si>
+    <t>Slight tap to motorbike</t>
+  </si>
+  <si>
+    <t>suv, motorbike</t>
+  </si>
+  <si>
+    <t>SUV seemed to hit the motorcyclist, toppling him over. No damage to the vehicles seemed to have been dealt, but the motorcyclist may need medical attention</t>
+  </si>
+  <si>
+    <t>Possibly</t>
+  </si>
+  <si>
+    <t>suv, sedan</t>
+  </si>
+  <si>
+    <t>One vehicle spun out and engine seen smoking - could lead to a fire in the future</t>
+  </si>
+  <si>
+    <t>Impact intensity is hard to determine, but definite t-bone collision happened</t>
+  </si>
+  <si>
+    <t>Day, close to sunrise/sunset</t>
+  </si>
+  <si>
+    <t>suv ran a red light and got hit, but it seems that both parties braked enough to not do serious damage</t>
+  </si>
+  <si>
+    <t>van, sedan</t>
+  </si>
+  <si>
+    <t>The side of the car hit was near the rear</t>
+  </si>
+  <si>
+    <t>sedan, 18-wheeler</t>
+  </si>
+  <si>
+    <t>sedan hits the rear of 18-wheeler</t>
+  </si>
+  <si>
+    <t>Impact intensity seemed very high - both parties are probably injured</t>
+  </si>
+  <si>
+    <t>happened at mildly busy intersection</t>
+  </si>
+  <si>
+    <t>No clear impact</t>
+  </si>
+  <si>
+    <t>motorbike, van</t>
+  </si>
+  <si>
+    <t>Motorcyclist reacted to van and fell off bike. However, no impact seemed to have been made</t>
+  </si>
+  <si>
+    <t>2 (possibly more?)</t>
+  </si>
+  <si>
+    <t>police sedan, truck</t>
+  </si>
+  <si>
+    <t>Day, possibly rainy?</t>
+  </si>
+  <si>
+    <t>Truck rear ends police car and spins on interstate, potentially affecting many other vehicles</t>
+  </si>
+  <si>
+    <t>suv x2, sedan</t>
+  </si>
+  <si>
+    <t>suv runs red light and gets hit by other two vehicles - light impact</t>
+  </si>
+  <si>
+    <t>Rear-end</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Sedan, Truck</t>
+  </si>
+  <si>
+    <t>truck was stopped and sedan was going too fast into a stop</t>
+  </si>
+  <si>
+    <t>Read-end</t>
+  </si>
+  <si>
+    <t>sedan, bus</t>
+  </si>
+  <si>
+    <t>Night, possibly hard to see</t>
+  </si>
+  <si>
+    <t>sedan crashes into bus that was not moving</t>
+  </si>
+  <si>
+    <t>Light tap into spin-out</t>
+  </si>
+  <si>
+    <t>sedan, truck</t>
+  </si>
+  <si>
+    <t>truck lightly taps sedan on roundabout into spinning out</t>
+  </si>
+  <si>
+    <t>spin-out</t>
+  </si>
+  <si>
+    <t>1 (possibly more?)</t>
+  </si>
+  <si>
+    <t>suv?</t>
+  </si>
+  <si>
+    <t>suv seems to spin out, but unclear if any other impact happened in the footage</t>
+  </si>
+  <si>
+    <t>Front-end</t>
+  </si>
+  <si>
+    <t>sedan seemed to be on wrong side of the road</t>
+  </si>
+  <si>
+    <t>T-bone into spin-out</t>
+  </si>
+  <si>
+    <t>sedan, 18-wheeler?</t>
+  </si>
+  <si>
+    <t>sedan runs into truck and spins the truck out in the intersection</t>
+  </si>
+  <si>
+    <t>t-bone</t>
+  </si>
+  <si>
+    <t>sedan x2?</t>
+  </si>
+  <si>
+    <t>happened at a busy intersection</t>
+  </si>
+  <si>
+    <t>Sedan, truck</t>
+  </si>
+  <si>
+    <t>Sedan t-bones truck</t>
+  </si>
+  <si>
+    <t>topple</t>
+  </si>
+  <si>
+    <t>truck</t>
+  </si>
+  <si>
+    <t>Truck seems to topple over, cause unknown, debris present</t>
+  </si>
+  <si>
+    <t>bus, sedan x4, suv x2</t>
+  </si>
+  <si>
+    <t>7 (possibly more)</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>bus crashes into sedan, resulting in snowball effect of collisions</t>
+  </si>
+  <si>
+    <t>van, 18-wheeler</t>
+  </si>
+  <si>
+    <t>Both vehicles spin out, and one vehicle is seen smoking from the engine</t>
+  </si>
+  <si>
+    <t>Topple</t>
+  </si>
+  <si>
+    <t>truck seemed to have spun out and toppled over, but the cause is unknown. Debris present</t>
+  </si>
+  <si>
+    <t>18-wheeler, sedan</t>
+  </si>
+  <si>
+    <t>18-wheeler hits sedan at intersection, smoke is present</t>
+  </si>
+  <si>
+    <t>day, cloudy?</t>
+  </si>
+  <si>
+    <t>Collision looks to have happened at an intersection</t>
+  </si>
+  <si>
+    <t>front-end</t>
+  </si>
+  <si>
+    <t>bus, 18-wheeler, sedan</t>
+  </si>
+  <si>
+    <t>Bus hits 18-wheeler and sedan slightly at a left turn</t>
+  </si>
+  <si>
+    <t>light t-bone</t>
+  </si>
+  <si>
+    <t>truck, bike</t>
+  </si>
+  <si>
+    <t>truck lightly hits cyclist, toppling him over</t>
+  </si>
+  <si>
+    <t>suv, motorcycle</t>
+  </si>
+  <si>
+    <t>Suv crashes into motorcyclist, leading to debris. Motorcyclist needs medical attention</t>
+  </si>
+  <si>
+    <t>cause unknown</t>
+  </si>
+  <si>
+    <t>sedan, ??</t>
+  </si>
+  <si>
+    <t>footage cannot determine what happened, but sedan's bumper and front seemed damaged at intersection</t>
+  </si>
+  <si>
+    <t>Although a side collision, impact still seemed great. A sign was destroyed in the process, and debris is present</t>
+  </si>
+  <si>
+    <t>suv, police sedan</t>
+  </si>
+  <si>
+    <t>suv crashes into police sedan (that was stopped) at an intersection</t>
+  </si>
+  <si>
+    <t>Suv, bike</t>
+  </si>
+  <si>
+    <t>Suv and bicyclist crash. Although cyclist was seem walking, medical attention is needed. Happened at busy area</t>
+  </si>
+  <si>
+    <t>Light tap, front side on front side</t>
+  </si>
+  <si>
+    <t>suv x2</t>
+  </si>
+  <si>
+    <t>Day, possibly cloudy</t>
+  </si>
+  <si>
+    <t>Both suvs seemed to lightly tap each other on the intersection</t>
   </si>
 </sst>
 </file>
@@ -522,10 +807,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,6 +1276,1368 @@
         <v>45</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" t="s">
+        <v>54</v>
+      </c>
+      <c r="K19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
+        <v>61</v>
+      </c>
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" t="s">
+        <v>64</v>
+      </c>
+      <c r="K22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>66</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" t="s">
+        <v>43</v>
+      </c>
+      <c r="K24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" t="s">
+        <v>68</v>
+      </c>
+      <c r="I25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" t="s">
+        <v>61</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" t="s">
+        <v>43</v>
+      </c>
+      <c r="K27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>43</v>
+      </c>
+      <c r="K28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" t="s">
+        <v>76</v>
+      </c>
+      <c r="I29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" t="s">
+        <v>77</v>
+      </c>
+      <c r="K29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" t="s">
+        <v>43</v>
+      </c>
+      <c r="K30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>29</v>
+      </c>
+      <c r="B31" s="3">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" t="s">
+        <v>82</v>
+      </c>
+      <c r="H31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" t="s">
+        <v>43</v>
+      </c>
+      <c r="K31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" t="s">
+        <v>86</v>
+      </c>
+      <c r="I32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" t="s">
+        <v>87</v>
+      </c>
+      <c r="K32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>31</v>
+      </c>
+      <c r="B33" s="3">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" t="s">
+        <v>90</v>
+      </c>
+      <c r="I33" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" t="s">
+        <v>43</v>
+      </c>
+      <c r="K33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>33</v>
+      </c>
+      <c r="B35" s="3">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" t="s">
+        <v>43</v>
+      </c>
+      <c r="K35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" t="s">
+        <v>27</v>
+      </c>
+      <c r="I36" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" t="s">
+        <v>26</v>
+      </c>
+      <c r="K36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>35</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" t="s">
+        <v>102</v>
+      </c>
+      <c r="I37" t="s">
+        <v>11</v>
+      </c>
+      <c r="J37" t="s">
+        <v>43</v>
+      </c>
+      <c r="K37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" t="s">
+        <v>104</v>
+      </c>
+      <c r="I38" t="s">
+        <v>11</v>
+      </c>
+      <c r="J38" t="s">
+        <v>43</v>
+      </c>
+      <c r="K38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>37</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" t="s">
+        <v>107</v>
+      </c>
+      <c r="I39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" t="s">
+        <v>43</v>
+      </c>
+      <c r="K39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>38</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" t="s">
+        <v>109</v>
+      </c>
+      <c r="I40" t="s">
+        <v>111</v>
+      </c>
+      <c r="J40" t="s">
+        <v>43</v>
+      </c>
+      <c r="K40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>39</v>
+      </c>
+      <c r="B41" s="3">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" t="s">
+        <v>113</v>
+      </c>
+      <c r="I41" t="s">
+        <v>82</v>
+      </c>
+      <c r="J41" t="s">
+        <v>43</v>
+      </c>
+      <c r="K41" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" t="s">
+        <v>107</v>
+      </c>
+      <c r="I42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J42" t="s">
+        <v>43</v>
+      </c>
+      <c r="K42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>41</v>
+      </c>
+      <c r="B43" s="3">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" t="s">
+        <v>82</v>
+      </c>
+      <c r="H43" t="s">
+        <v>117</v>
+      </c>
+      <c r="I43" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43" t="s">
+        <v>26</v>
+      </c>
+      <c r="K43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>42</v>
+      </c>
+      <c r="B44" s="3">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D44" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" t="s">
+        <v>61</v>
+      </c>
+      <c r="I44" t="s">
+        <v>11</v>
+      </c>
+      <c r="J44" t="s">
+        <v>119</v>
+      </c>
+      <c r="K44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>43</v>
+      </c>
+      <c r="B45" s="3">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" t="s">
+        <v>122</v>
+      </c>
+      <c r="I45" t="s">
+        <v>11</v>
+      </c>
+      <c r="J45" t="s">
+        <v>43</v>
+      </c>
+      <c r="K45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>44</v>
+      </c>
+      <c r="B46" s="3">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" t="s">
+        <v>125</v>
+      </c>
+      <c r="I46" t="s">
+        <v>11</v>
+      </c>
+      <c r="J46" t="s">
+        <v>37</v>
+      </c>
+      <c r="K46" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>45</v>
+      </c>
+      <c r="B47" s="3">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" t="s">
+        <v>127</v>
+      </c>
+      <c r="I47" t="s">
+        <v>11</v>
+      </c>
+      <c r="J47" t="s">
+        <v>37</v>
+      </c>
+      <c r="K47" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" t="s">
+        <v>129</v>
+      </c>
+      <c r="D48" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" t="s">
+        <v>130</v>
+      </c>
+      <c r="I48" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48" t="s">
+        <v>37</v>
+      </c>
+      <c r="K48" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>47</v>
+      </c>
+      <c r="B49" s="3">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" t="s">
+        <v>61</v>
+      </c>
+      <c r="I49" t="s">
+        <v>11</v>
+      </c>
+      <c r="J49" t="s">
+        <v>37</v>
+      </c>
+      <c r="K49" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>48</v>
+      </c>
+      <c r="B50" s="3">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" t="s">
+        <v>133</v>
+      </c>
+      <c r="I50" t="s">
+        <v>11</v>
+      </c>
+      <c r="J50" t="s">
+        <v>43</v>
+      </c>
+      <c r="K50" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>49</v>
+      </c>
+      <c r="B51" s="3">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" t="s">
+        <v>15</v>
+      </c>
+      <c r="H51" t="s">
+        <v>135</v>
+      </c>
+      <c r="I51" t="s">
+        <v>11</v>
+      </c>
+      <c r="J51" t="s">
+        <v>43</v>
+      </c>
+      <c r="K51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>50</v>
+      </c>
+      <c r="B52" s="3">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" t="s">
+        <v>15</v>
+      </c>
+      <c r="H52" t="s">
+        <v>138</v>
+      </c>
+      <c r="I52" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" t="s">
+        <v>139</v>
+      </c>
+      <c r="K52" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added up to 82
</commit_message>
<xml_diff>
--- a/accident_ground_truths.xlsx
+++ b/accident_ground_truths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5671703E-7049-4032-A39B-6F10C41755ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A739C7D7-E182-44EF-A628-3A79B760473F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="205">
   <si>
     <t>Number of vehicles in accident</t>
   </si>
@@ -443,6 +443,198 @@
   </si>
   <si>
     <t>Both suvs seemed to lightly tap each other on the intersection</t>
+  </si>
+  <si>
+    <t>light tap into side</t>
+  </si>
+  <si>
+    <t>sedan, bike</t>
+  </si>
+  <si>
+    <t>Cyclist hits the sedan at an intersection lightly</t>
+  </si>
+  <si>
+    <t>industrial truck x2</t>
+  </si>
+  <si>
+    <t>Happened at an intersection</t>
+  </si>
+  <si>
+    <t>t-bone (angled)</t>
+  </si>
+  <si>
+    <t>18-wheeler, suv</t>
+  </si>
+  <si>
+    <t>Truck is seen smoking, happened at vacant intersection</t>
+  </si>
+  <si>
+    <t>Light tap in intersection</t>
+  </si>
+  <si>
+    <t>van, motorbike</t>
+  </si>
+  <si>
+    <t>Light tap from van to motorcyclist, toppling motorcyclist</t>
+  </si>
+  <si>
+    <t>light tap</t>
+  </si>
+  <si>
+    <t>truck, sedan</t>
+  </si>
+  <si>
+    <t>Light tap from truck, accident did not seem very serious</t>
+  </si>
+  <si>
+    <t>taxi sedan, sedan</t>
+  </si>
+  <si>
+    <t>Strong hit at busy intersection</t>
+  </si>
+  <si>
+    <t>Multiple passengers were in one vehicle, accident was clearly shown to stop a lot of traffic immediately</t>
+  </si>
+  <si>
+    <t>Cloudy day?</t>
+  </si>
+  <si>
+    <t>Truck hits sedan and drags the sedan off the road - serious damage occurred</t>
+  </si>
+  <si>
+    <t>T-bone (high speed)</t>
+  </si>
+  <si>
+    <t>Sedan that was at fault was definitely speeding here - high impact</t>
+  </si>
+  <si>
+    <t>sedan, police sedan</t>
+  </si>
+  <si>
+    <t>Police car had lights on and hit sedan that seemed to be unaware of this</t>
+  </si>
+  <si>
+    <t>rear-end</t>
+  </si>
+  <si>
+    <t>sedan, van</t>
+  </si>
+  <si>
+    <t>sedan hits van strongly at a light</t>
+  </si>
+  <si>
+    <t>van x2</t>
+  </si>
+  <si>
+    <t>Day, snowy</t>
+  </si>
+  <si>
+    <t>t-bone (light tap)</t>
+  </si>
+  <si>
+    <t>it looks that one van lost control and went straight thru the intersection, resulting in the other van hitting it</t>
+  </si>
+  <si>
+    <t>Night, snowy</t>
+  </si>
+  <si>
+    <t>probably was caused by lack of control</t>
+  </si>
+  <si>
+    <t>car against pedestrian</t>
+  </si>
+  <si>
+    <t>suv</t>
+  </si>
+  <si>
+    <t>Car hits pedestrian extremely hard - medical attention is vital</t>
+  </si>
+  <si>
+    <t>18-wheeler x2, sedan x2</t>
+  </si>
+  <si>
+    <t>day, clear</t>
+  </si>
+  <si>
+    <t>One rear end collision leads to domino effect</t>
+  </si>
+  <si>
+    <t>18-wheeler, train</t>
+  </si>
+  <si>
+    <t>Train hits 18-wheeler's trailer, so no person injuries but lots of debris</t>
+  </si>
+  <si>
+    <t>1 (maybe more?)</t>
+  </si>
+  <si>
+    <t>spin-out?</t>
+  </si>
+  <si>
+    <t>Truck loses control and crashes into a parking lot - unclear whether or not other vehicles were hit</t>
+  </si>
+  <si>
+    <t>angled t-bone?</t>
+  </si>
+  <si>
+    <t>van, buggy?</t>
+  </si>
+  <si>
+    <t>Van crashes into small "buggy" and topples it over</t>
+  </si>
+  <si>
+    <t>van, bus</t>
+  </si>
+  <si>
+    <t>Bus t-bones van at intersection that is mildly busy</t>
+  </si>
+  <si>
+    <t>bus x2</t>
+  </si>
+  <si>
+    <t>Bus rear-ends anotheer bus at large straightaway</t>
+  </si>
+  <si>
+    <t>t-bone?</t>
+  </si>
+  <si>
+    <t>sedan, bike?</t>
+  </si>
+  <si>
+    <t>It's hard to tell from the footage, but it seems that a sedan either hit a bike or a pedestrian at an intersection</t>
+  </si>
+  <si>
+    <t>It looks like a sedan hit a bike, but footage is too grainy to tell</t>
+  </si>
+  <si>
+    <t>Person seemed to have ejected from one of the vehicles in the midst of the collision</t>
+  </si>
+  <si>
+    <t>Truck topples over whilst crossing an intersection</t>
+  </si>
+  <si>
+    <t>Sedan topples over cyclist</t>
+  </si>
+  <si>
+    <t>bus, bike</t>
+  </si>
+  <si>
+    <t>Bus hits biker and topples the biker - it is likely that medical attention is needed</t>
+  </si>
+  <si>
+    <t>scooter</t>
+  </si>
+  <si>
+    <t>Scooter topples over in intersection. It seems that the user can just pick up and carry on. Nothing should be necessary</t>
+  </si>
+  <si>
+    <t>bike</t>
+  </si>
+  <si>
+    <t>bike seemed to have toppled over before the time of the footage, but this small accident was cleaned up before anything serious happened</t>
+  </si>
+  <si>
+    <t>scooter seemed to topple over, but no harm seemed to have been done</t>
   </si>
 </sst>
 </file>
@@ -807,10 +999,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2638,6 +2830,1126 @@
         <v>140</v>
       </c>
     </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>51</v>
+      </c>
+      <c r="B53" s="3">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>141</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" t="s">
+        <v>142</v>
+      </c>
+      <c r="I53" t="s">
+        <v>11</v>
+      </c>
+      <c r="J53" t="s">
+        <v>43</v>
+      </c>
+      <c r="K53" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54" s="3">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" t="s">
+        <v>15</v>
+      </c>
+      <c r="H54" t="s">
+        <v>61</v>
+      </c>
+      <c r="I54" t="s">
+        <v>11</v>
+      </c>
+      <c r="J54" t="s">
+        <v>54</v>
+      </c>
+      <c r="K54" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>53</v>
+      </c>
+      <c r="B55" s="3">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>146</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" t="s">
+        <v>144</v>
+      </c>
+      <c r="I55" t="s">
+        <v>11</v>
+      </c>
+      <c r="J55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K55" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>54</v>
+      </c>
+      <c r="B56" s="3">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>146</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" t="s">
+        <v>15</v>
+      </c>
+      <c r="G56" t="s">
+        <v>15</v>
+      </c>
+      <c r="H56" t="s">
+        <v>147</v>
+      </c>
+      <c r="I56" t="s">
+        <v>15</v>
+      </c>
+      <c r="J56" t="s">
+        <v>54</v>
+      </c>
+      <c r="K56" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>55</v>
+      </c>
+      <c r="B57" s="3">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" t="s">
+        <v>46</v>
+      </c>
+      <c r="I57" t="s">
+        <v>11</v>
+      </c>
+      <c r="J57" t="s">
+        <v>37</v>
+      </c>
+      <c r="K57" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>56</v>
+      </c>
+      <c r="B58" s="3">
+        <v>2</v>
+      </c>
+      <c r="C58" t="s">
+        <v>124</v>
+      </c>
+      <c r="D58" t="s">
+        <v>60</v>
+      </c>
+      <c r="E58" t="s">
+        <v>60</v>
+      </c>
+      <c r="F58" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" t="s">
+        <v>15</v>
+      </c>
+      <c r="H58" t="s">
+        <v>150</v>
+      </c>
+      <c r="I58" t="s">
+        <v>11</v>
+      </c>
+      <c r="J58" t="s">
+        <v>43</v>
+      </c>
+      <c r="K58" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>57</v>
+      </c>
+      <c r="B59" s="3">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>152</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" t="s">
+        <v>153</v>
+      </c>
+      <c r="I59" t="s">
+        <v>11</v>
+      </c>
+      <c r="J59" t="s">
+        <v>26</v>
+      </c>
+      <c r="K59" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>58</v>
+      </c>
+      <c r="B60" s="3">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>146</v>
+      </c>
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" t="s">
+        <v>11</v>
+      </c>
+      <c r="G60" t="s">
+        <v>15</v>
+      </c>
+      <c r="H60" t="s">
+        <v>155</v>
+      </c>
+      <c r="I60" t="s">
+        <v>11</v>
+      </c>
+      <c r="J60" t="s">
+        <v>26</v>
+      </c>
+      <c r="K60" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>59</v>
+      </c>
+      <c r="B61" s="3">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" t="s">
+        <v>11</v>
+      </c>
+      <c r="G61" t="s">
+        <v>15</v>
+      </c>
+      <c r="H61" t="s">
+        <v>46</v>
+      </c>
+      <c r="I61" t="s">
+        <v>11</v>
+      </c>
+      <c r="J61" t="s">
+        <v>26</v>
+      </c>
+      <c r="K61" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>60</v>
+      </c>
+      <c r="B62" s="3">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" t="s">
+        <v>82</v>
+      </c>
+      <c r="F62" t="s">
+        <v>11</v>
+      </c>
+      <c r="G62" t="s">
+        <v>15</v>
+      </c>
+      <c r="H62" t="s">
+        <v>46</v>
+      </c>
+      <c r="I62" t="s">
+        <v>11</v>
+      </c>
+      <c r="J62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K62" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>61</v>
+      </c>
+      <c r="B63" s="3">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" t="s">
+        <v>15</v>
+      </c>
+      <c r="G63" t="s">
+        <v>15</v>
+      </c>
+      <c r="H63" t="s">
+        <v>90</v>
+      </c>
+      <c r="I63" t="s">
+        <v>11</v>
+      </c>
+      <c r="J63" t="s">
+        <v>158</v>
+      </c>
+      <c r="K63" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>62</v>
+      </c>
+      <c r="B64" s="3">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>160</v>
+      </c>
+      <c r="D64" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" t="s">
+        <v>82</v>
+      </c>
+      <c r="F64" t="s">
+        <v>11</v>
+      </c>
+      <c r="G64" t="s">
+        <v>15</v>
+      </c>
+      <c r="H64" t="s">
+        <v>46</v>
+      </c>
+      <c r="I64" t="s">
+        <v>11</v>
+      </c>
+      <c r="J64" t="s">
+        <v>26</v>
+      </c>
+      <c r="K64" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>63</v>
+      </c>
+      <c r="B65" s="3">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" t="s">
+        <v>11</v>
+      </c>
+      <c r="G65" t="s">
+        <v>15</v>
+      </c>
+      <c r="H65" t="s">
+        <v>162</v>
+      </c>
+      <c r="I65" t="s">
+        <v>11</v>
+      </c>
+      <c r="J65" t="s">
+        <v>26</v>
+      </c>
+      <c r="K65" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>64</v>
+      </c>
+      <c r="B66" s="3">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>164</v>
+      </c>
+      <c r="D66" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66" t="s">
+        <v>11</v>
+      </c>
+      <c r="G66" t="s">
+        <v>15</v>
+      </c>
+      <c r="H66" t="s">
+        <v>165</v>
+      </c>
+      <c r="I66" t="s">
+        <v>11</v>
+      </c>
+      <c r="J66" t="s">
+        <v>26</v>
+      </c>
+      <c r="K66" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>65</v>
+      </c>
+      <c r="B67" s="3">
+        <v>2</v>
+      </c>
+      <c r="C67" t="s">
+        <v>169</v>
+      </c>
+      <c r="D67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" t="s">
+        <v>15</v>
+      </c>
+      <c r="H67" t="s">
+        <v>167</v>
+      </c>
+      <c r="I67" t="s">
+        <v>11</v>
+      </c>
+      <c r="J67" t="s">
+        <v>168</v>
+      </c>
+      <c r="K67" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>66</v>
+      </c>
+      <c r="B68" s="3">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D68" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68" t="s">
+        <v>15</v>
+      </c>
+      <c r="F68" t="s">
+        <v>11</v>
+      </c>
+      <c r="G68" t="s">
+        <v>15</v>
+      </c>
+      <c r="H68" t="s">
+        <v>138</v>
+      </c>
+      <c r="I68" t="s">
+        <v>11</v>
+      </c>
+      <c r="J68" t="s">
+        <v>171</v>
+      </c>
+      <c r="K68" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>67</v>
+      </c>
+      <c r="B69" s="3">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>173</v>
+      </c>
+      <c r="D69" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" t="s">
+        <v>15</v>
+      </c>
+      <c r="H69" t="s">
+        <v>174</v>
+      </c>
+      <c r="I69" t="s">
+        <v>11</v>
+      </c>
+      <c r="J69" t="s">
+        <v>26</v>
+      </c>
+      <c r="K69" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>68</v>
+      </c>
+      <c r="B70" s="3">
+        <v>4</v>
+      </c>
+      <c r="C70" t="s">
+        <v>164</v>
+      </c>
+      <c r="D70" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" t="s">
+        <v>15</v>
+      </c>
+      <c r="F70" t="s">
+        <v>11</v>
+      </c>
+      <c r="G70" t="s">
+        <v>15</v>
+      </c>
+      <c r="H70" t="s">
+        <v>176</v>
+      </c>
+      <c r="I70" t="s">
+        <v>11</v>
+      </c>
+      <c r="J70" t="s">
+        <v>177</v>
+      </c>
+      <c r="K70" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>69</v>
+      </c>
+      <c r="B71" s="3">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>101</v>
+      </c>
+      <c r="D71" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71" t="s">
+        <v>11</v>
+      </c>
+      <c r="G71" t="s">
+        <v>15</v>
+      </c>
+      <c r="H71" t="s">
+        <v>179</v>
+      </c>
+      <c r="I71" t="s">
+        <v>11</v>
+      </c>
+      <c r="J71" t="s">
+        <v>37</v>
+      </c>
+      <c r="K71" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>70</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C72" t="s">
+        <v>182</v>
+      </c>
+      <c r="D72" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" t="s">
+        <v>11</v>
+      </c>
+      <c r="G72" t="s">
+        <v>15</v>
+      </c>
+      <c r="H72" t="s">
+        <v>107</v>
+      </c>
+      <c r="I72" t="s">
+        <v>11</v>
+      </c>
+      <c r="J72" t="s">
+        <v>37</v>
+      </c>
+      <c r="K72" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>71</v>
+      </c>
+      <c r="B73" s="3">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>184</v>
+      </c>
+      <c r="D73" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" t="s">
+        <v>15</v>
+      </c>
+      <c r="F73" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73" t="s">
+        <v>15</v>
+      </c>
+      <c r="H73" t="s">
+        <v>185</v>
+      </c>
+      <c r="I73" t="s">
+        <v>11</v>
+      </c>
+      <c r="J73" t="s">
+        <v>37</v>
+      </c>
+      <c r="K73" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>72</v>
+      </c>
+      <c r="B74" s="3">
+        <v>2</v>
+      </c>
+      <c r="C74" t="s">
+        <v>101</v>
+      </c>
+      <c r="D74" t="s">
+        <v>15</v>
+      </c>
+      <c r="E74" t="s">
+        <v>15</v>
+      </c>
+      <c r="F74" t="s">
+        <v>11</v>
+      </c>
+      <c r="G74" t="s">
+        <v>15</v>
+      </c>
+      <c r="H74" t="s">
+        <v>187</v>
+      </c>
+      <c r="I74" t="s">
+        <v>11</v>
+      </c>
+      <c r="J74" t="s">
+        <v>37</v>
+      </c>
+      <c r="K74" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>73</v>
+      </c>
+      <c r="B75" s="3">
+        <v>2</v>
+      </c>
+      <c r="C75" t="s">
+        <v>164</v>
+      </c>
+      <c r="D75" t="s">
+        <v>60</v>
+      </c>
+      <c r="E75" t="s">
+        <v>60</v>
+      </c>
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75" t="s">
+        <v>15</v>
+      </c>
+      <c r="H75" t="s">
+        <v>189</v>
+      </c>
+      <c r="I75" t="s">
+        <v>11</v>
+      </c>
+      <c r="J75" t="s">
+        <v>37</v>
+      </c>
+      <c r="K75" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>74</v>
+      </c>
+      <c r="B76" s="3">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
+        <v>191</v>
+      </c>
+      <c r="D76" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" t="s">
+        <v>15</v>
+      </c>
+      <c r="F76" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76" t="s">
+        <v>15</v>
+      </c>
+      <c r="H76" t="s">
+        <v>192</v>
+      </c>
+      <c r="I76" t="s">
+        <v>11</v>
+      </c>
+      <c r="J76" t="s">
+        <v>26</v>
+      </c>
+      <c r="K76" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <v>75</v>
+      </c>
+      <c r="B77" s="3">
+        <v>2</v>
+      </c>
+      <c r="C77" t="s">
+        <v>129</v>
+      </c>
+      <c r="D77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" t="s">
+        <v>11</v>
+      </c>
+      <c r="F77" t="s">
+        <v>11</v>
+      </c>
+      <c r="G77" t="s">
+        <v>11</v>
+      </c>
+      <c r="H77" t="s">
+        <v>192</v>
+      </c>
+      <c r="I77" t="s">
+        <v>11</v>
+      </c>
+      <c r="J77" t="s">
+        <v>37</v>
+      </c>
+      <c r="K77" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>76</v>
+      </c>
+      <c r="B78" s="3">
+        <v>2</v>
+      </c>
+      <c r="C78" t="s">
+        <v>49</v>
+      </c>
+      <c r="D78" t="s">
+        <v>15</v>
+      </c>
+      <c r="E78" t="s">
+        <v>15</v>
+      </c>
+      <c r="F78" t="s">
+        <v>11</v>
+      </c>
+      <c r="G78" t="s">
+        <v>15</v>
+      </c>
+      <c r="H78" t="s">
+        <v>46</v>
+      </c>
+      <c r="I78" t="s">
+        <v>11</v>
+      </c>
+      <c r="J78" t="s">
+        <v>37</v>
+      </c>
+      <c r="K78" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>77</v>
+      </c>
+      <c r="B79" s="3">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>106</v>
+      </c>
+      <c r="D79" t="s">
+        <v>15</v>
+      </c>
+      <c r="E79" t="s">
+        <v>15</v>
+      </c>
+      <c r="F79" t="s">
+        <v>11</v>
+      </c>
+      <c r="G79" t="s">
+        <v>15</v>
+      </c>
+      <c r="H79" t="s">
+        <v>107</v>
+      </c>
+      <c r="I79" t="s">
+        <v>11</v>
+      </c>
+      <c r="J79" t="s">
+        <v>26</v>
+      </c>
+      <c r="K79" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
+        <v>78</v>
+      </c>
+      <c r="B80" s="3">
+        <v>2</v>
+      </c>
+      <c r="C80" t="s">
+        <v>49</v>
+      </c>
+      <c r="D80" t="s">
+        <v>15</v>
+      </c>
+      <c r="E80" t="s">
+        <v>15</v>
+      </c>
+      <c r="F80" t="s">
+        <v>11</v>
+      </c>
+      <c r="G80" t="s">
+        <v>15</v>
+      </c>
+      <c r="H80" t="s">
+        <v>142</v>
+      </c>
+      <c r="I80" t="s">
+        <v>11</v>
+      </c>
+      <c r="J80" t="s">
+        <v>26</v>
+      </c>
+      <c r="K80" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
+        <v>79</v>
+      </c>
+      <c r="B81" s="3">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>101</v>
+      </c>
+      <c r="D81" t="s">
+        <v>15</v>
+      </c>
+      <c r="E81" t="s">
+        <v>15</v>
+      </c>
+      <c r="F81" t="s">
+        <v>11</v>
+      </c>
+      <c r="G81" t="s">
+        <v>15</v>
+      </c>
+      <c r="H81" t="s">
+        <v>198</v>
+      </c>
+      <c r="I81" t="s">
+        <v>11</v>
+      </c>
+      <c r="J81" t="s">
+        <v>37</v>
+      </c>
+      <c r="K81" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <v>80</v>
+      </c>
+      <c r="B82" s="3">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>106</v>
+      </c>
+      <c r="D82" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" t="s">
+        <v>11</v>
+      </c>
+      <c r="G82" t="s">
+        <v>11</v>
+      </c>
+      <c r="H82" t="s">
+        <v>200</v>
+      </c>
+      <c r="I82" t="s">
+        <v>11</v>
+      </c>
+      <c r="J82" t="s">
+        <v>37</v>
+      </c>
+      <c r="K82" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <v>81</v>
+      </c>
+      <c r="B83" s="3">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>129</v>
+      </c>
+      <c r="D83" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" t="s">
+        <v>11</v>
+      </c>
+      <c r="G83" t="s">
+        <v>11</v>
+      </c>
+      <c r="H83" t="s">
+        <v>202</v>
+      </c>
+      <c r="I83" t="s">
+        <v>11</v>
+      </c>
+      <c r="J83" t="s">
+        <v>177</v>
+      </c>
+      <c r="K83" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <v>82</v>
+      </c>
+      <c r="B84" s="3">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>129</v>
+      </c>
+      <c r="D84" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G84" t="s">
+        <v>11</v>
+      </c>
+      <c r="H84" t="s">
+        <v>200</v>
+      </c>
+      <c r="I84" t="s">
+        <v>11</v>
+      </c>
+      <c r="J84" t="s">
+        <v>37</v>
+      </c>
+      <c r="K84" t="s">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Feb 20 Meeting fixes to sheet
</commit_message>
<xml_diff>
--- a/accident_ground_truths.xlsx
+++ b/accident_ground_truths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A739C7D7-E182-44EF-A628-3A79B760473F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F452BFF1-8572-4660-91A6-986F028977AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="206">
   <si>
     <t>Number of vehicles in accident</t>
   </si>
@@ -635,6 +635,9 @@
   </si>
   <si>
     <t>scooter seemed to topple over, but no harm seemed to have been done</t>
+  </si>
+  <si>
+    <t>Low Res/Bad Footage?</t>
   </si>
 </sst>
 </file>
@@ -999,10 +1002,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K84"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1021,7 @@
     <col min="9" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1048,10 +1051,13 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
+        <v>205</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1083,10 +1089,13 @@
         <v>12</v>
       </c>
       <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1118,10 +1127,13 @@
         <v>17</v>
       </c>
       <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1153,10 +1165,13 @@
         <v>21</v>
       </c>
       <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1188,10 +1203,13 @@
         <v>21</v>
       </c>
       <c r="K5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1223,10 +1241,13 @@
         <v>26</v>
       </c>
       <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1258,10 +1279,13 @@
         <v>26</v>
       </c>
       <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1293,10 +1317,13 @@
         <v>26</v>
       </c>
       <c r="K8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1328,10 +1355,13 @@
         <v>26</v>
       </c>
       <c r="K9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1363,10 +1393,13 @@
         <v>37</v>
       </c>
       <c r="K10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1398,10 +1431,13 @@
         <v>40</v>
       </c>
       <c r="K11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1432,8 +1468,11 @@
       <c r="J12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1465,10 +1504,13 @@
         <v>43</v>
       </c>
       <c r="K13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1500,10 +1542,13 @@
         <v>47</v>
       </c>
       <c r="K14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1535,10 +1580,13 @@
         <v>43</v>
       </c>
       <c r="K15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1570,10 +1618,13 @@
         <v>52</v>
       </c>
       <c r="K16" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1605,10 +1656,13 @@
         <v>26</v>
       </c>
       <c r="K17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1640,10 +1694,13 @@
         <v>54</v>
       </c>
       <c r="K18" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1675,10 +1732,13 @@
         <v>54</v>
       </c>
       <c r="K19" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1695,7 +1755,7 @@
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="G20" t="s">
         <v>15</v>
@@ -1710,10 +1770,13 @@
         <v>26</v>
       </c>
       <c r="K20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1745,10 +1808,13 @@
         <v>26</v>
       </c>
       <c r="K21" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1780,10 +1846,13 @@
         <v>64</v>
       </c>
       <c r="K22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1814,8 +1883,11 @@
       <c r="J23" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -1847,10 +1919,13 @@
         <v>43</v>
       </c>
       <c r="K24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -1861,10 +1936,10 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
@@ -1882,10 +1957,13 @@
         <v>26</v>
       </c>
       <c r="K25" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -1917,10 +1995,13 @@
         <v>43</v>
       </c>
       <c r="K26" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -1952,10 +2033,13 @@
         <v>43</v>
       </c>
       <c r="K27" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -1987,10 +2071,13 @@
         <v>43</v>
       </c>
       <c r="K28" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -2022,10 +2109,13 @@
         <v>77</v>
       </c>
       <c r="K29" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -2057,10 +2147,13 @@
         <v>43</v>
       </c>
       <c r="K30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L30" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -2074,7 +2167,7 @@
         <v>60</v>
       </c>
       <c r="E31" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="F31" t="s">
         <v>11</v>
@@ -2092,10 +2185,13 @@
         <v>43</v>
       </c>
       <c r="K31" t="s">
+        <v>11</v>
+      </c>
+      <c r="L31" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -2127,10 +2223,13 @@
         <v>87</v>
       </c>
       <c r="K32" t="s">
+        <v>11</v>
+      </c>
+      <c r="L32" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -2162,10 +2261,13 @@
         <v>43</v>
       </c>
       <c r="K33" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -2196,11 +2298,14 @@
       <c r="J34" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="K34" t="s">
+        <v>15</v>
+      </c>
+      <c r="L34" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2232,10 +2337,13 @@
         <v>43</v>
       </c>
       <c r="K35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L35" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -2267,10 +2375,13 @@
         <v>26</v>
       </c>
       <c r="K36" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -2302,10 +2413,13 @@
         <v>43</v>
       </c>
       <c r="K37" t="s">
+        <v>11</v>
+      </c>
+      <c r="L37" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -2337,10 +2451,13 @@
         <v>43</v>
       </c>
       <c r="K38" t="s">
+        <v>11</v>
+      </c>
+      <c r="L38" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -2372,10 +2489,13 @@
         <v>43</v>
       </c>
       <c r="K39" t="s">
+        <v>11</v>
+      </c>
+      <c r="L39" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -2407,10 +2527,13 @@
         <v>43</v>
       </c>
       <c r="K40" t="s">
+        <v>11</v>
+      </c>
+      <c r="L40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -2442,10 +2565,13 @@
         <v>43</v>
       </c>
       <c r="K41" t="s">
+        <v>11</v>
+      </c>
+      <c r="L41" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>40</v>
       </c>
@@ -2477,10 +2603,13 @@
         <v>43</v>
       </c>
       <c r="K42" t="s">
+        <v>11</v>
+      </c>
+      <c r="L42" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -2512,10 +2641,13 @@
         <v>26</v>
       </c>
       <c r="K43" t="s">
+        <v>11</v>
+      </c>
+      <c r="L43" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -2547,10 +2679,13 @@
         <v>119</v>
       </c>
       <c r="K44" t="s">
+        <v>11</v>
+      </c>
+      <c r="L44" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -2582,10 +2717,13 @@
         <v>43</v>
       </c>
       <c r="K45" t="s">
+        <v>11</v>
+      </c>
+      <c r="L45" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -2617,10 +2755,13 @@
         <v>37</v>
       </c>
       <c r="K46" t="s">
+        <v>11</v>
+      </c>
+      <c r="L46" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -2652,10 +2793,13 @@
         <v>37</v>
       </c>
       <c r="K47" t="s">
+        <v>11</v>
+      </c>
+      <c r="L47" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -2669,7 +2813,7 @@
         <v>60</v>
       </c>
       <c r="E48" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="F48" t="s">
         <v>11</v>
@@ -2687,10 +2831,13 @@
         <v>37</v>
       </c>
       <c r="K48" t="s">
+        <v>15</v>
+      </c>
+      <c r="L48" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -2722,10 +2869,13 @@
         <v>37</v>
       </c>
       <c r="K49" t="s">
+        <v>11</v>
+      </c>
+      <c r="L49" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>48</v>
       </c>
@@ -2757,10 +2907,13 @@
         <v>43</v>
       </c>
       <c r="K50" t="s">
+        <v>11</v>
+      </c>
+      <c r="L50" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>49</v>
       </c>
@@ -2792,10 +2945,13 @@
         <v>43</v>
       </c>
       <c r="K51" t="s">
+        <v>11</v>
+      </c>
+      <c r="L51" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -2827,10 +2983,13 @@
         <v>139</v>
       </c>
       <c r="K52" t="s">
+        <v>11</v>
+      </c>
+      <c r="L52" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -2862,10 +3021,13 @@
         <v>43</v>
       </c>
       <c r="K53" t="s">
+        <v>11</v>
+      </c>
+      <c r="L53" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -2897,10 +3059,13 @@
         <v>54</v>
       </c>
       <c r="K54" t="s">
+        <v>11</v>
+      </c>
+      <c r="L54" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -2932,10 +3097,13 @@
         <v>54</v>
       </c>
       <c r="K55" t="s">
+        <v>11</v>
+      </c>
+      <c r="L55" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>54</v>
       </c>
@@ -2967,10 +3135,13 @@
         <v>54</v>
       </c>
       <c r="K56" t="s">
+        <v>11</v>
+      </c>
+      <c r="L56" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>55</v>
       </c>
@@ -3002,10 +3173,13 @@
         <v>37</v>
       </c>
       <c r="K57" t="s">
+        <v>11</v>
+      </c>
+      <c r="L57" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>56</v>
       </c>
@@ -3019,7 +3193,7 @@
         <v>60</v>
       </c>
       <c r="E58" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="F58" t="s">
         <v>11</v>
@@ -3037,10 +3211,13 @@
         <v>43</v>
       </c>
       <c r="K58" t="s">
+        <v>11</v>
+      </c>
+      <c r="L58" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>57</v>
       </c>
@@ -3072,10 +3249,13 @@
         <v>26</v>
       </c>
       <c r="K59" t="s">
+        <v>11</v>
+      </c>
+      <c r="L59" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>58</v>
       </c>
@@ -3107,10 +3287,13 @@
         <v>26</v>
       </c>
       <c r="K60" t="s">
+        <v>11</v>
+      </c>
+      <c r="L60" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -3142,10 +3325,13 @@
         <v>26</v>
       </c>
       <c r="K61" t="s">
+        <v>11</v>
+      </c>
+      <c r="L61" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>60</v>
       </c>
@@ -3177,10 +3363,13 @@
         <v>26</v>
       </c>
       <c r="K62" t="s">
+        <v>11</v>
+      </c>
+      <c r="L62" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -3212,10 +3401,13 @@
         <v>158</v>
       </c>
       <c r="K63" t="s">
+        <v>11</v>
+      </c>
+      <c r="L63" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>62</v>
       </c>
@@ -3247,10 +3439,13 @@
         <v>26</v>
       </c>
       <c r="K64" t="s">
+        <v>11</v>
+      </c>
+      <c r="L64" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -3282,10 +3477,13 @@
         <v>26</v>
       </c>
       <c r="K65" t="s">
+        <v>11</v>
+      </c>
+      <c r="L65" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>64</v>
       </c>
@@ -3317,10 +3515,13 @@
         <v>26</v>
       </c>
       <c r="K66" t="s">
+        <v>11</v>
+      </c>
+      <c r="L66" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>65</v>
       </c>
@@ -3352,10 +3553,13 @@
         <v>168</v>
       </c>
       <c r="K67" t="s">
+        <v>11</v>
+      </c>
+      <c r="L67" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>66</v>
       </c>
@@ -3387,10 +3591,13 @@
         <v>171</v>
       </c>
       <c r="K68" t="s">
+        <v>11</v>
+      </c>
+      <c r="L68" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>67</v>
       </c>
@@ -3422,10 +3629,13 @@
         <v>26</v>
       </c>
       <c r="K69" t="s">
+        <v>11</v>
+      </c>
+      <c r="L69" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>68</v>
       </c>
@@ -3457,10 +3667,13 @@
         <v>177</v>
       </c>
       <c r="K70" t="s">
+        <v>11</v>
+      </c>
+      <c r="L70" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>69</v>
       </c>
@@ -3492,10 +3705,13 @@
         <v>37</v>
       </c>
       <c r="K71" t="s">
+        <v>11</v>
+      </c>
+      <c r="L71" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>70</v>
       </c>
@@ -3527,10 +3743,13 @@
         <v>37</v>
       </c>
       <c r="K72" t="s">
+        <v>11</v>
+      </c>
+      <c r="L72" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>71</v>
       </c>
@@ -3562,10 +3781,13 @@
         <v>37</v>
       </c>
       <c r="K73" t="s">
+        <v>11</v>
+      </c>
+      <c r="L73" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>72</v>
       </c>
@@ -3597,10 +3819,13 @@
         <v>37</v>
       </c>
       <c r="K74" t="s">
+        <v>11</v>
+      </c>
+      <c r="L74" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>73</v>
       </c>
@@ -3614,7 +3839,7 @@
         <v>60</v>
       </c>
       <c r="E75" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="F75" t="s">
         <v>11</v>
@@ -3632,10 +3857,13 @@
         <v>37</v>
       </c>
       <c r="K75" t="s">
+        <v>11</v>
+      </c>
+      <c r="L75" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>74</v>
       </c>
@@ -3667,10 +3895,13 @@
         <v>26</v>
       </c>
       <c r="K76" t="s">
+        <v>11</v>
+      </c>
+      <c r="L76" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>75</v>
       </c>
@@ -3702,10 +3933,13 @@
         <v>37</v>
       </c>
       <c r="K77" t="s">
+        <v>15</v>
+      </c>
+      <c r="L77" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>76</v>
       </c>
@@ -3737,10 +3971,13 @@
         <v>37</v>
       </c>
       <c r="K78" t="s">
+        <v>11</v>
+      </c>
+      <c r="L78" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>77</v>
       </c>
@@ -3772,10 +4009,13 @@
         <v>26</v>
       </c>
       <c r="K79" t="s">
+        <v>11</v>
+      </c>
+      <c r="L79" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>78</v>
       </c>
@@ -3807,10 +4047,13 @@
         <v>26</v>
       </c>
       <c r="K80" t="s">
+        <v>11</v>
+      </c>
+      <c r="L80" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>79</v>
       </c>
@@ -3842,10 +4085,13 @@
         <v>37</v>
       </c>
       <c r="K81" t="s">
+        <v>11</v>
+      </c>
+      <c r="L81" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>80</v>
       </c>
@@ -3877,10 +4123,13 @@
         <v>37</v>
       </c>
       <c r="K82" t="s">
+        <v>11</v>
+      </c>
+      <c r="L82" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>81</v>
       </c>
@@ -3912,10 +4161,13 @@
         <v>177</v>
       </c>
       <c r="K83" t="s">
+        <v>11</v>
+      </c>
+      <c r="L83" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>82</v>
       </c>
@@ -3947,6 +4199,9 @@
         <v>37</v>
       </c>
       <c r="K84" t="s">
+        <v>11</v>
+      </c>
+      <c r="L84" t="s">
         <v>204</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added up to 101
</commit_message>
<xml_diff>
--- a/accident_ground_truths.xlsx
+++ b/accident_ground_truths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F452BFF1-8572-4660-91A6-986F028977AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6DC5CB-6896-434F-9F17-807314272EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="241">
   <si>
     <t>Number of vehicles in accident</t>
   </si>
@@ -638,6 +638,111 @@
   </si>
   <si>
     <t>Low Res/Bad Footage?</t>
+  </si>
+  <si>
+    <t>t-bone (angled0</t>
+  </si>
+  <si>
+    <t>collision happened at 2 lane road</t>
+  </si>
+  <si>
+    <t>bus, van</t>
+  </si>
+  <si>
+    <t>happened at congested area, so there could be more involved in the accident</t>
+  </si>
+  <si>
+    <t>scooter?</t>
+  </si>
+  <si>
+    <t>Although the cause is unknown, it seems that a bike toppled over at an intersection</t>
+  </si>
+  <si>
+    <t>bus, sedan</t>
+  </si>
+  <si>
+    <t>There don't seem to be many streetlights here, so it was hard to see specific vehicles</t>
+  </si>
+  <si>
+    <t>sedan, scooter</t>
+  </si>
+  <si>
+    <t>Nobody seemed to be hurt by the end. Happened close to an intersection</t>
+  </si>
+  <si>
+    <t>Happened at a busy intersection, mild impact</t>
+  </si>
+  <si>
+    <t>motorbike</t>
+  </si>
+  <si>
+    <t>Simple topple at an intersection, nothing to be done</t>
+  </si>
+  <si>
+    <t>bus, motorbike</t>
+  </si>
+  <si>
+    <t>Although light impact, motorcyclist probably needs medical attention</t>
+  </si>
+  <si>
+    <t>buggy?, motorbike</t>
+  </si>
+  <si>
+    <t>It doesn't look like anyone was hurt, but send over police just in case</t>
+  </si>
+  <si>
+    <t>18-wheeler</t>
+  </si>
+  <si>
+    <t>18-wheeler took a sharp turn and toppled - debris present and damage to city inflicted</t>
+  </si>
+  <si>
+    <t>bike, truck</t>
+  </si>
+  <si>
+    <t>Bike hits truck lightly. Cyclist can like just get up and move on</t>
+  </si>
+  <si>
+    <t>2 (likely more)</t>
+  </si>
+  <si>
+    <t>18-wheeler topples on interstate and hits other vehicles in the process. Debris present. Maximum assistance is needed</t>
+  </si>
+  <si>
+    <t>18-wheeler (again) topples on interstate and hits other vehicles in the process. Debris present. Maximum assistance is needed</t>
+  </si>
+  <si>
+    <t>18-wheeler, van</t>
+  </si>
+  <si>
+    <t>Day, rainy</t>
+  </si>
+  <si>
+    <t>happened at intersection, light impact</t>
+  </si>
+  <si>
+    <t>bike, suv</t>
+  </si>
+  <si>
+    <t>Rainy, cloudy day</t>
+  </si>
+  <si>
+    <t>Suv hits cyclist - cyclist could be injured so medical assistance is necessary</t>
+  </si>
+  <si>
+    <t>suv, bus</t>
+  </si>
+  <si>
+    <t>suv ran a red light and hit the bus lightly</t>
+  </si>
+  <si>
+    <t>light/mild rear end collision near a traffic light</t>
+  </si>
+  <si>
+    <t>bike, 18-wheeler?</t>
+  </si>
+  <si>
+    <t>big vehicle looks to have run a red light and, as a result, the biker hits the vehicle</t>
   </si>
 </sst>
 </file>
@@ -1002,10 +1107,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L84"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="E73" workbookViewId="0">
+      <selection activeCell="L103" sqref="L103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4205,6 +4310,728 @@
         <v>204</v>
       </c>
     </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <v>83</v>
+      </c>
+      <c r="B85" s="3">
+        <v>2</v>
+      </c>
+      <c r="C85" t="s">
+        <v>206</v>
+      </c>
+      <c r="D85" t="s">
+        <v>60</v>
+      </c>
+      <c r="E85" t="s">
+        <v>15</v>
+      </c>
+      <c r="F85" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" t="s">
+        <v>15</v>
+      </c>
+      <c r="H85" t="s">
+        <v>24</v>
+      </c>
+      <c r="I85" t="s">
+        <v>11</v>
+      </c>
+      <c r="J85" t="s">
+        <v>26</v>
+      </c>
+      <c r="K85" t="s">
+        <v>11</v>
+      </c>
+      <c r="L85" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
+        <v>84</v>
+      </c>
+      <c r="B86" s="3">
+        <v>2</v>
+      </c>
+      <c r="C86" t="s">
+        <v>164</v>
+      </c>
+      <c r="D86" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" t="s">
+        <v>11</v>
+      </c>
+      <c r="F86" t="s">
+        <v>11</v>
+      </c>
+      <c r="G86" t="s">
+        <v>15</v>
+      </c>
+      <c r="H86" t="s">
+        <v>208</v>
+      </c>
+      <c r="I86" t="s">
+        <v>11</v>
+      </c>
+      <c r="J86" t="s">
+        <v>43</v>
+      </c>
+      <c r="K86" t="s">
+        <v>11</v>
+      </c>
+      <c r="L86" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="3">
+        <v>85</v>
+      </c>
+      <c r="B87" s="3">
+        <v>1</v>
+      </c>
+      <c r="C87" t="s">
+        <v>129</v>
+      </c>
+      <c r="D87" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87" t="s">
+        <v>11</v>
+      </c>
+      <c r="F87" t="s">
+        <v>11</v>
+      </c>
+      <c r="G87" t="s">
+        <v>11</v>
+      </c>
+      <c r="H87" t="s">
+        <v>210</v>
+      </c>
+      <c r="I87" t="s">
+        <v>11</v>
+      </c>
+      <c r="J87" t="s">
+        <v>43</v>
+      </c>
+      <c r="K87" t="s">
+        <v>15</v>
+      </c>
+      <c r="L87" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
+        <v>86</v>
+      </c>
+      <c r="B88" s="3">
+        <v>2</v>
+      </c>
+      <c r="C88" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" t="s">
+        <v>15</v>
+      </c>
+      <c r="E88" t="s">
+        <v>15</v>
+      </c>
+      <c r="F88" t="s">
+        <v>11</v>
+      </c>
+      <c r="G88" t="s">
+        <v>15</v>
+      </c>
+      <c r="H88" t="s">
+        <v>212</v>
+      </c>
+      <c r="I88" t="s">
+        <v>11</v>
+      </c>
+      <c r="J88" t="s">
+        <v>26</v>
+      </c>
+      <c r="K88" t="s">
+        <v>11</v>
+      </c>
+      <c r="L88" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="3">
+        <v>87</v>
+      </c>
+      <c r="B89" s="3">
+        <v>2</v>
+      </c>
+      <c r="C89" t="s">
+        <v>164</v>
+      </c>
+      <c r="D89" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" t="s">
+        <v>11</v>
+      </c>
+      <c r="G89" t="s">
+        <v>15</v>
+      </c>
+      <c r="H89" t="s">
+        <v>214</v>
+      </c>
+      <c r="I89" t="s">
+        <v>11</v>
+      </c>
+      <c r="J89" t="s">
+        <v>43</v>
+      </c>
+      <c r="K89" t="s">
+        <v>11</v>
+      </c>
+      <c r="L89" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="3">
+        <v>88</v>
+      </c>
+      <c r="B90" s="3">
+        <v>2</v>
+      </c>
+      <c r="C90" t="s">
+        <v>23</v>
+      </c>
+      <c r="D90" t="s">
+        <v>15</v>
+      </c>
+      <c r="E90" t="s">
+        <v>15</v>
+      </c>
+      <c r="F90" t="s">
+        <v>11</v>
+      </c>
+      <c r="G90" t="s">
+        <v>15</v>
+      </c>
+      <c r="H90" t="s">
+        <v>138</v>
+      </c>
+      <c r="I90" t="s">
+        <v>11</v>
+      </c>
+      <c r="J90" t="s">
+        <v>43</v>
+      </c>
+      <c r="K90" t="s">
+        <v>11</v>
+      </c>
+      <c r="L90" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
+        <v>89</v>
+      </c>
+      <c r="B91" s="3">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>106</v>
+      </c>
+      <c r="D91" t="s">
+        <v>11</v>
+      </c>
+      <c r="E91" t="s">
+        <v>11</v>
+      </c>
+      <c r="F91" t="s">
+        <v>11</v>
+      </c>
+      <c r="G91" t="s">
+        <v>11</v>
+      </c>
+      <c r="H91" t="s">
+        <v>217</v>
+      </c>
+      <c r="I91" t="s">
+        <v>11</v>
+      </c>
+      <c r="J91" t="s">
+        <v>43</v>
+      </c>
+      <c r="K91" t="s">
+        <v>11</v>
+      </c>
+      <c r="L91" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
+        <v>90</v>
+      </c>
+      <c r="B92" s="3">
+        <v>2</v>
+      </c>
+      <c r="C92" t="s">
+        <v>124</v>
+      </c>
+      <c r="D92" t="s">
+        <v>15</v>
+      </c>
+      <c r="E92" t="s">
+        <v>15</v>
+      </c>
+      <c r="F92" t="s">
+        <v>11</v>
+      </c>
+      <c r="G92" t="s">
+        <v>15</v>
+      </c>
+      <c r="H92" t="s">
+        <v>219</v>
+      </c>
+      <c r="I92" t="s">
+        <v>11</v>
+      </c>
+      <c r="J92" t="s">
+        <v>43</v>
+      </c>
+      <c r="K92" t="s">
+        <v>11</v>
+      </c>
+      <c r="L92" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
+        <v>91</v>
+      </c>
+      <c r="B93" s="3">
+        <v>2</v>
+      </c>
+      <c r="C93" t="s">
+        <v>124</v>
+      </c>
+      <c r="D93" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93" t="s">
+        <v>11</v>
+      </c>
+      <c r="F93" t="s">
+        <v>11</v>
+      </c>
+      <c r="G93" t="s">
+        <v>15</v>
+      </c>
+      <c r="H93" t="s">
+        <v>221</v>
+      </c>
+      <c r="I93" t="s">
+        <v>11</v>
+      </c>
+      <c r="J93" t="s">
+        <v>43</v>
+      </c>
+      <c r="K93" t="s">
+        <v>11</v>
+      </c>
+      <c r="L93" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
+        <v>92</v>
+      </c>
+      <c r="B94" s="3">
+        <v>1</v>
+      </c>
+      <c r="C94" t="s">
+        <v>106</v>
+      </c>
+      <c r="D94" t="s">
+        <v>15</v>
+      </c>
+      <c r="E94" t="s">
+        <v>15</v>
+      </c>
+      <c r="F94" t="s">
+        <v>11</v>
+      </c>
+      <c r="G94" t="s">
+        <v>15</v>
+      </c>
+      <c r="H94" t="s">
+        <v>223</v>
+      </c>
+      <c r="I94" t="s">
+        <v>11</v>
+      </c>
+      <c r="J94" t="s">
+        <v>43</v>
+      </c>
+      <c r="K94" t="s">
+        <v>11</v>
+      </c>
+      <c r="L94" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="3">
+        <v>93</v>
+      </c>
+      <c r="B95" s="3">
+        <v>1</v>
+      </c>
+      <c r="C95" t="s">
+        <v>164</v>
+      </c>
+      <c r="D95" t="s">
+        <v>11</v>
+      </c>
+      <c r="E95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F95" t="s">
+        <v>11</v>
+      </c>
+      <c r="G95" t="s">
+        <v>11</v>
+      </c>
+      <c r="H95" t="s">
+        <v>225</v>
+      </c>
+      <c r="I95" t="s">
+        <v>11</v>
+      </c>
+      <c r="J95" t="s">
+        <v>43</v>
+      </c>
+      <c r="K95" t="s">
+        <v>11</v>
+      </c>
+      <c r="L95" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="3">
+        <v>94</v>
+      </c>
+      <c r="B96" s="3">
+        <v>0</v>
+      </c>
+      <c r="C96" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96" t="s">
+        <v>11</v>
+      </c>
+      <c r="E96" t="s">
+        <v>11</v>
+      </c>
+      <c r="F96" t="s">
+        <v>11</v>
+      </c>
+      <c r="G96" t="s">
+        <v>11</v>
+      </c>
+      <c r="H96" t="s">
+        <v>10</v>
+      </c>
+      <c r="I96" t="s">
+        <v>11</v>
+      </c>
+      <c r="J96" t="s">
+        <v>37</v>
+      </c>
+      <c r="K96" t="s">
+        <v>11</v>
+      </c>
+      <c r="L96" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="3">
+        <v>95</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C97" t="s">
+        <v>106</v>
+      </c>
+      <c r="D97" t="s">
+        <v>15</v>
+      </c>
+      <c r="E97" t="s">
+        <v>15</v>
+      </c>
+      <c r="F97" t="s">
+        <v>15</v>
+      </c>
+      <c r="G97" t="s">
+        <v>15</v>
+      </c>
+      <c r="H97" t="s">
+        <v>117</v>
+      </c>
+      <c r="I97" t="s">
+        <v>11</v>
+      </c>
+      <c r="J97" t="s">
+        <v>54</v>
+      </c>
+      <c r="K97" t="s">
+        <v>11</v>
+      </c>
+      <c r="L97" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="3">
+        <v>96</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C98" t="s">
+        <v>106</v>
+      </c>
+      <c r="D98" t="s">
+        <v>15</v>
+      </c>
+      <c r="E98" t="s">
+        <v>15</v>
+      </c>
+      <c r="F98" t="s">
+        <v>15</v>
+      </c>
+      <c r="G98" t="s">
+        <v>15</v>
+      </c>
+      <c r="H98" t="s">
+        <v>117</v>
+      </c>
+      <c r="I98" t="s">
+        <v>11</v>
+      </c>
+      <c r="J98" t="s">
+        <v>54</v>
+      </c>
+      <c r="K98" t="s">
+        <v>11</v>
+      </c>
+      <c r="L98" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="3">
+        <v>97</v>
+      </c>
+      <c r="B99" s="3">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
+        <v>124</v>
+      </c>
+      <c r="D99" t="s">
+        <v>11</v>
+      </c>
+      <c r="E99" t="s">
+        <v>11</v>
+      </c>
+      <c r="F99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G99" t="s">
+        <v>15</v>
+      </c>
+      <c r="H99" t="s">
+        <v>230</v>
+      </c>
+      <c r="I99" t="s">
+        <v>11</v>
+      </c>
+      <c r="J99" t="s">
+        <v>231</v>
+      </c>
+      <c r="K99" t="s">
+        <v>11</v>
+      </c>
+      <c r="L99" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="3">
+        <v>98</v>
+      </c>
+      <c r="B100" s="3">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
+        <v>124</v>
+      </c>
+      <c r="D100" t="s">
+        <v>60</v>
+      </c>
+      <c r="E100" t="s">
+        <v>15</v>
+      </c>
+      <c r="F100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G100" t="s">
+        <v>15</v>
+      </c>
+      <c r="H100" t="s">
+        <v>233</v>
+      </c>
+      <c r="I100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J100" t="s">
+        <v>234</v>
+      </c>
+      <c r="K100" t="s">
+        <v>11</v>
+      </c>
+      <c r="L100" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="3">
+        <v>99</v>
+      </c>
+      <c r="B101" s="3">
+        <v>2</v>
+      </c>
+      <c r="C101" t="s">
+        <v>146</v>
+      </c>
+      <c r="D101" t="s">
+        <v>11</v>
+      </c>
+      <c r="E101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F101" t="s">
+        <v>11</v>
+      </c>
+      <c r="G101" t="s">
+        <v>15</v>
+      </c>
+      <c r="H101" t="s">
+        <v>236</v>
+      </c>
+      <c r="I101" t="s">
+        <v>11</v>
+      </c>
+      <c r="J101" t="s">
+        <v>26</v>
+      </c>
+      <c r="K101" t="s">
+        <v>11</v>
+      </c>
+      <c r="L101" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="3">
+        <v>100</v>
+      </c>
+      <c r="B102" s="3">
+        <v>2</v>
+      </c>
+      <c r="C102" t="s">
+        <v>164</v>
+      </c>
+      <c r="D102" t="s">
+        <v>11</v>
+      </c>
+      <c r="E102" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" t="s">
+        <v>11</v>
+      </c>
+      <c r="G102" t="s">
+        <v>15</v>
+      </c>
+      <c r="H102" t="s">
+        <v>138</v>
+      </c>
+      <c r="I102" t="s">
+        <v>11</v>
+      </c>
+      <c r="J102" t="s">
+        <v>234</v>
+      </c>
+      <c r="K102" t="s">
+        <v>11</v>
+      </c>
+      <c r="L102" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" s="3">
+        <v>101</v>
+      </c>
+      <c r="B103" s="3">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>101</v>
+      </c>
+      <c r="D103" t="s">
+        <v>15</v>
+      </c>
+      <c r="E103" t="s">
+        <v>15</v>
+      </c>
+      <c r="F103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G103" t="s">
+        <v>15</v>
+      </c>
+      <c r="H103" t="s">
+        <v>239</v>
+      </c>
+      <c r="I103" t="s">
+        <v>11</v>
+      </c>
+      <c r="J103" t="s">
+        <v>158</v>
+      </c>
+      <c r="K103" t="s">
+        <v>11</v>
+      </c>
+      <c r="L103" t="s">
+        <v>240</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
first accuracy matrix + program
</commit_message>
<xml_diff>
--- a/accident_ground_truths.xlsx
+++ b/accident_ground_truths.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6DC5CB-6896-434F-9F17-807314272EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB219C0F-936F-4AE6-92DF-9897AFAA3101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16275" yWindow="0" windowWidth="12630" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="240">
   <si>
     <t>Number of vehicles in accident</t>
   </si>
@@ -275,9 +275,6 @@
   </si>
   <si>
     <t>truck was stopped and sedan was going too fast into a stop</t>
-  </si>
-  <si>
-    <t>Read-end</t>
   </si>
   <si>
     <t>sedan, bus</t>
@@ -1109,8 +1106,8 @@
   </sheetPr>
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E73" workbookViewId="0">
-      <selection activeCell="L103" sqref="L103"/>
+    <sheetView tabSelected="1" topLeftCell="G94" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,7 +1153,7 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -2304,7 +2301,7 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
         <v>82</v>
@@ -2319,19 +2316,19 @@
         <v>15</v>
       </c>
       <c r="H32" t="s">
+        <v>85</v>
+      </c>
+      <c r="I32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" t="s">
         <v>86</v>
       </c>
-      <c r="I32" t="s">
-        <v>11</v>
-      </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
+        <v>11</v>
+      </c>
+      <c r="L32" t="s">
         <v>87</v>
-      </c>
-      <c r="K32" t="s">
-        <v>11</v>
-      </c>
-      <c r="L32" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2342,22 +2339,22 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" t="s">
         <v>89</v>
-      </c>
-      <c r="D33" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" t="s">
-        <v>90</v>
       </c>
       <c r="I33" t="s">
         <v>11</v>
@@ -2369,7 +2366,7 @@
         <v>11</v>
       </c>
       <c r="L33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2377,25 +2374,25 @@
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>11</v>
@@ -2407,7 +2404,7 @@
         <v>15</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2418,7 +2415,7 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D35" t="s">
         <v>15</v>
@@ -2433,7 +2430,7 @@
         <v>15</v>
       </c>
       <c r="H35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I35" t="s">
         <v>11</v>
@@ -2445,7 +2442,7 @@
         <v>11</v>
       </c>
       <c r="L35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2456,7 +2453,7 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D36" t="s">
         <v>15</v>
@@ -2483,7 +2480,7 @@
         <v>11</v>
       </c>
       <c r="L36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2494,22 +2491,22 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" t="s">
         <v>101</v>
-      </c>
-      <c r="D37" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" t="s">
-        <v>11</v>
-      </c>
-      <c r="G37" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" t="s">
-        <v>102</v>
       </c>
       <c r="I37" t="s">
         <v>11</v>
@@ -2521,7 +2518,7 @@
         <v>11</v>
       </c>
       <c r="L37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2532,7 +2529,7 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -2547,7 +2544,7 @@
         <v>15</v>
       </c>
       <c r="H38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I38" t="s">
         <v>11</v>
@@ -2559,7 +2556,7 @@
         <v>11</v>
       </c>
       <c r="L38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2570,22 +2567,22 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" t="s">
         <v>106</v>
-      </c>
-      <c r="D39" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" t="s">
-        <v>107</v>
       </c>
       <c r="I39" t="s">
         <v>11</v>
@@ -2597,7 +2594,7 @@
         <v>11</v>
       </c>
       <c r="L39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2605,28 +2602,28 @@
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" t="s">
+        <v>108</v>
+      </c>
+      <c r="I40" t="s">
         <v>110</v>
-      </c>
-      <c r="C40" t="s">
-        <v>101</v>
-      </c>
-      <c r="D40" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40" t="s">
-        <v>15</v>
-      </c>
-      <c r="F40" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H40" t="s">
-        <v>109</v>
-      </c>
-      <c r="I40" t="s">
-        <v>111</v>
       </c>
       <c r="J40" t="s">
         <v>43</v>
@@ -2635,7 +2632,7 @@
         <v>11</v>
       </c>
       <c r="L40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2646,7 +2643,7 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D41" t="s">
         <v>15</v>
@@ -2661,7 +2658,7 @@
         <v>15</v>
       </c>
       <c r="H41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I41" t="s">
         <v>82</v>
@@ -2673,7 +2670,7 @@
         <v>11</v>
       </c>
       <c r="L41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2684,7 +2681,7 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D42" t="s">
         <v>15</v>
@@ -2699,7 +2696,7 @@
         <v>15</v>
       </c>
       <c r="H42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I42" t="s">
         <v>11</v>
@@ -2711,7 +2708,7 @@
         <v>11</v>
       </c>
       <c r="L42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2737,7 +2734,7 @@
         <v>82</v>
       </c>
       <c r="H43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I43" t="s">
         <v>15</v>
@@ -2749,7 +2746,7 @@
         <v>11</v>
       </c>
       <c r="L43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2760,7 +2757,7 @@
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D44" t="s">
         <v>15</v>
@@ -2781,13 +2778,13 @@
         <v>11</v>
       </c>
       <c r="J44" t="s">
+        <v>118</v>
+      </c>
+      <c r="K44" t="s">
+        <v>11</v>
+      </c>
+      <c r="L44" t="s">
         <v>119</v>
-      </c>
-      <c r="K44" t="s">
-        <v>11</v>
-      </c>
-      <c r="L44" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2798,7 +2795,7 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D45" t="s">
         <v>82</v>
@@ -2813,7 +2810,7 @@
         <v>15</v>
       </c>
       <c r="H45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I45" t="s">
         <v>11</v>
@@ -2825,7 +2822,7 @@
         <v>11</v>
       </c>
       <c r="L45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2836,22 +2833,22 @@
         <v>2</v>
       </c>
       <c r="C46" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" t="s">
         <v>124</v>
-      </c>
-      <c r="D46" t="s">
-        <v>15</v>
-      </c>
-      <c r="E46" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" t="s">
-        <v>15</v>
-      </c>
-      <c r="H46" t="s">
-        <v>125</v>
       </c>
       <c r="I46" t="s">
         <v>11</v>
@@ -2863,7 +2860,7 @@
         <v>11</v>
       </c>
       <c r="L46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2874,7 +2871,7 @@
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D47" t="s">
         <v>15</v>
@@ -2889,7 +2886,7 @@
         <v>15</v>
       </c>
       <c r="H47" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I47" t="s">
         <v>11</v>
@@ -2901,7 +2898,7 @@
         <v>11</v>
       </c>
       <c r="L47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2909,10 +2906,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C48" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D48" t="s">
         <v>60</v>
@@ -2927,7 +2924,7 @@
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I48" t="s">
         <v>11</v>
@@ -2939,7 +2936,7 @@
         <v>15</v>
       </c>
       <c r="L48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2977,7 +2974,7 @@
         <v>11</v>
       </c>
       <c r="L49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -3003,7 +3000,7 @@
         <v>15</v>
       </c>
       <c r="H50" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I50" t="s">
         <v>11</v>
@@ -3015,7 +3012,7 @@
         <v>11</v>
       </c>
       <c r="L50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3026,7 +3023,7 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D51" t="s">
         <v>15</v>
@@ -3041,7 +3038,7 @@
         <v>15</v>
       </c>
       <c r="H51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I51" t="s">
         <v>11</v>
@@ -3053,7 +3050,7 @@
         <v>11</v>
       </c>
       <c r="L51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -3064,34 +3061,34 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" t="s">
+        <v>15</v>
+      </c>
+      <c r="H52" t="s">
         <v>137</v>
       </c>
-      <c r="D52" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" t="s">
-        <v>11</v>
-      </c>
-      <c r="G52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" t="s">
         <v>138</v>
       </c>
-      <c r="I52" t="s">
-        <v>11</v>
-      </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
+        <v>11</v>
+      </c>
+      <c r="L52" t="s">
         <v>139</v>
-      </c>
-      <c r="K52" t="s">
-        <v>11</v>
-      </c>
-      <c r="L52" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3102,22 +3099,22 @@
         <v>2</v>
       </c>
       <c r="C53" t="s">
+        <v>140</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" t="s">
         <v>141</v>
-      </c>
-      <c r="D53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" t="s">
-        <v>11</v>
-      </c>
-      <c r="G53" t="s">
-        <v>11</v>
-      </c>
-      <c r="H53" t="s">
-        <v>142</v>
       </c>
       <c r="I53" t="s">
         <v>11</v>
@@ -3129,7 +3126,7 @@
         <v>11</v>
       </c>
       <c r="L53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3140,7 +3137,7 @@
         <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D54" t="s">
         <v>15</v>
@@ -3167,7 +3164,7 @@
         <v>11</v>
       </c>
       <c r="L54" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3178,7 +3175,7 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -3193,7 +3190,7 @@
         <v>15</v>
       </c>
       <c r="H55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I55" t="s">
         <v>11</v>
@@ -3205,7 +3202,7 @@
         <v>11</v>
       </c>
       <c r="L55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -3216,22 +3213,22 @@
         <v>2</v>
       </c>
       <c r="C56" t="s">
+        <v>145</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" t="s">
+        <v>15</v>
+      </c>
+      <c r="G56" t="s">
+        <v>15</v>
+      </c>
+      <c r="H56" t="s">
         <v>146</v>
-      </c>
-      <c r="D56" t="s">
-        <v>15</v>
-      </c>
-      <c r="E56" t="s">
-        <v>15</v>
-      </c>
-      <c r="F56" t="s">
-        <v>15</v>
-      </c>
-      <c r="G56" t="s">
-        <v>15</v>
-      </c>
-      <c r="H56" t="s">
-        <v>147</v>
       </c>
       <c r="I56" t="s">
         <v>15</v>
@@ -3243,7 +3240,7 @@
         <v>11</v>
       </c>
       <c r="L56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -3254,7 +3251,7 @@
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D57" t="s">
         <v>11</v>
@@ -3281,7 +3278,7 @@
         <v>11</v>
       </c>
       <c r="L57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -3292,7 +3289,7 @@
         <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D58" t="s">
         <v>60</v>
@@ -3307,7 +3304,7 @@
         <v>15</v>
       </c>
       <c r="H58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I58" t="s">
         <v>11</v>
@@ -3319,7 +3316,7 @@
         <v>11</v>
       </c>
       <c r="L58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -3330,22 +3327,22 @@
         <v>2</v>
       </c>
       <c r="C59" t="s">
+        <v>151</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" t="s">
         <v>152</v>
-      </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" t="s">
-        <v>11</v>
-      </c>
-      <c r="G59" t="s">
-        <v>11</v>
-      </c>
-      <c r="H59" t="s">
-        <v>153</v>
       </c>
       <c r="I59" t="s">
         <v>11</v>
@@ -3357,7 +3354,7 @@
         <v>11</v>
       </c>
       <c r="L59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -3368,7 +3365,7 @@
         <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D60" t="s">
         <v>15</v>
@@ -3383,7 +3380,7 @@
         <v>15</v>
       </c>
       <c r="H60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I60" t="s">
         <v>11</v>
@@ -3395,7 +3392,7 @@
         <v>11</v>
       </c>
       <c r="L60" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -3433,7 +3430,7 @@
         <v>11</v>
       </c>
       <c r="L61" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -3471,7 +3468,7 @@
         <v>11</v>
       </c>
       <c r="L62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -3497,19 +3494,19 @@
         <v>15</v>
       </c>
       <c r="H63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I63" t="s">
         <v>11</v>
       </c>
       <c r="J63" t="s">
+        <v>157</v>
+      </c>
+      <c r="K63" t="s">
+        <v>11</v>
+      </c>
+      <c r="L63" t="s">
         <v>158</v>
-      </c>
-      <c r="K63" t="s">
-        <v>11</v>
-      </c>
-      <c r="L63" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -3520,7 +3517,7 @@
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D64" t="s">
         <v>15</v>
@@ -3547,7 +3544,7 @@
         <v>11</v>
       </c>
       <c r="L64" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -3573,7 +3570,7 @@
         <v>15</v>
       </c>
       <c r="H65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I65" t="s">
         <v>11</v>
@@ -3585,7 +3582,7 @@
         <v>11</v>
       </c>
       <c r="L65" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -3596,22 +3593,22 @@
         <v>2</v>
       </c>
       <c r="C66" t="s">
+        <v>163</v>
+      </c>
+      <c r="D66" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66" t="s">
+        <v>11</v>
+      </c>
+      <c r="G66" t="s">
+        <v>15</v>
+      </c>
+      <c r="H66" t="s">
         <v>164</v>
-      </c>
-      <c r="D66" t="s">
-        <v>15</v>
-      </c>
-      <c r="E66" t="s">
-        <v>15</v>
-      </c>
-      <c r="F66" t="s">
-        <v>11</v>
-      </c>
-      <c r="G66" t="s">
-        <v>15</v>
-      </c>
-      <c r="H66" t="s">
-        <v>165</v>
       </c>
       <c r="I66" t="s">
         <v>11</v>
@@ -3623,7 +3620,7 @@
         <v>11</v>
       </c>
       <c r="L66" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -3634,34 +3631,34 @@
         <v>2</v>
       </c>
       <c r="C67" t="s">
+        <v>168</v>
+      </c>
+      <c r="D67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" t="s">
+        <v>15</v>
+      </c>
+      <c r="H67" t="s">
+        <v>166</v>
+      </c>
+      <c r="I67" t="s">
+        <v>11</v>
+      </c>
+      <c r="J67" t="s">
+        <v>167</v>
+      </c>
+      <c r="K67" t="s">
+        <v>11</v>
+      </c>
+      <c r="L67" t="s">
         <v>169</v>
-      </c>
-      <c r="D67" t="s">
-        <v>15</v>
-      </c>
-      <c r="E67" t="s">
-        <v>15</v>
-      </c>
-      <c r="F67" t="s">
-        <v>11</v>
-      </c>
-      <c r="G67" t="s">
-        <v>15</v>
-      </c>
-      <c r="H67" t="s">
-        <v>167</v>
-      </c>
-      <c r="I67" t="s">
-        <v>11</v>
-      </c>
-      <c r="J67" t="s">
-        <v>168</v>
-      </c>
-      <c r="K67" t="s">
-        <v>11</v>
-      </c>
-      <c r="L67" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -3672,7 +3669,7 @@
         <v>2</v>
       </c>
       <c r="C68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D68" t="s">
         <v>15</v>
@@ -3687,19 +3684,19 @@
         <v>15</v>
       </c>
       <c r="H68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I68" t="s">
         <v>11</v>
       </c>
       <c r="J68" t="s">
+        <v>170</v>
+      </c>
+      <c r="K68" t="s">
+        <v>11</v>
+      </c>
+      <c r="L68" t="s">
         <v>171</v>
-      </c>
-      <c r="K68" t="s">
-        <v>11</v>
-      </c>
-      <c r="L68" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -3710,22 +3707,22 @@
         <v>1</v>
       </c>
       <c r="C69" t="s">
+        <v>172</v>
+      </c>
+      <c r="D69" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" t="s">
+        <v>15</v>
+      </c>
+      <c r="H69" t="s">
         <v>173</v>
-      </c>
-      <c r="D69" t="s">
-        <v>15</v>
-      </c>
-      <c r="E69" t="s">
-        <v>15</v>
-      </c>
-      <c r="F69" t="s">
-        <v>11</v>
-      </c>
-      <c r="G69" t="s">
-        <v>15</v>
-      </c>
-      <c r="H69" t="s">
-        <v>174</v>
       </c>
       <c r="I69" t="s">
         <v>11</v>
@@ -3737,7 +3734,7 @@
         <v>11</v>
       </c>
       <c r="L69" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -3748,7 +3745,7 @@
         <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D70" t="s">
         <v>15</v>
@@ -3763,19 +3760,19 @@
         <v>15</v>
       </c>
       <c r="H70" t="s">
+        <v>175</v>
+      </c>
+      <c r="I70" t="s">
+        <v>11</v>
+      </c>
+      <c r="J70" t="s">
         <v>176</v>
       </c>
-      <c r="I70" t="s">
-        <v>11</v>
-      </c>
-      <c r="J70" t="s">
+      <c r="K70" t="s">
+        <v>11</v>
+      </c>
+      <c r="L70" t="s">
         <v>177</v>
-      </c>
-      <c r="K70" t="s">
-        <v>11</v>
-      </c>
-      <c r="L70" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -3786,7 +3783,7 @@
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D71" t="s">
         <v>11</v>
@@ -3801,7 +3798,7 @@
         <v>15</v>
       </c>
       <c r="H71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I71" t="s">
         <v>11</v>
@@ -3813,7 +3810,7 @@
         <v>11</v>
       </c>
       <c r="L71" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -3821,11 +3818,11 @@
         <v>70</v>
       </c>
       <c r="B72" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C72" t="s">
         <v>181</v>
       </c>
-      <c r="C72" t="s">
-        <v>182</v>
-      </c>
       <c r="D72" t="s">
         <v>11</v>
       </c>
@@ -3839,7 +3836,7 @@
         <v>15</v>
       </c>
       <c r="H72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I72" t="s">
         <v>11</v>
@@ -3851,7 +3848,7 @@
         <v>11</v>
       </c>
       <c r="L72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -3862,22 +3859,22 @@
         <v>2</v>
       </c>
       <c r="C73" t="s">
+        <v>183</v>
+      </c>
+      <c r="D73" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" t="s">
+        <v>15</v>
+      </c>
+      <c r="F73" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73" t="s">
+        <v>15</v>
+      </c>
+      <c r="H73" t="s">
         <v>184</v>
-      </c>
-      <c r="D73" t="s">
-        <v>15</v>
-      </c>
-      <c r="E73" t="s">
-        <v>15</v>
-      </c>
-      <c r="F73" t="s">
-        <v>11</v>
-      </c>
-      <c r="G73" t="s">
-        <v>15</v>
-      </c>
-      <c r="H73" t="s">
-        <v>185</v>
       </c>
       <c r="I73" t="s">
         <v>11</v>
@@ -3889,7 +3886,7 @@
         <v>11</v>
       </c>
       <c r="L73" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -3900,7 +3897,7 @@
         <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D74" t="s">
         <v>15</v>
@@ -3915,7 +3912,7 @@
         <v>15</v>
       </c>
       <c r="H74" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I74" t="s">
         <v>11</v>
@@ -3927,7 +3924,7 @@
         <v>11</v>
       </c>
       <c r="L74" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -3938,7 +3935,7 @@
         <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D75" t="s">
         <v>60</v>
@@ -3953,7 +3950,7 @@
         <v>15</v>
       </c>
       <c r="H75" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I75" t="s">
         <v>11</v>
@@ -3965,7 +3962,7 @@
         <v>11</v>
       </c>
       <c r="L75" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -3976,22 +3973,22 @@
         <v>2</v>
       </c>
       <c r="C76" t="s">
+        <v>190</v>
+      </c>
+      <c r="D76" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" t="s">
+        <v>15</v>
+      </c>
+      <c r="F76" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76" t="s">
+        <v>15</v>
+      </c>
+      <c r="H76" t="s">
         <v>191</v>
-      </c>
-      <c r="D76" t="s">
-        <v>15</v>
-      </c>
-      <c r="E76" t="s">
-        <v>15</v>
-      </c>
-      <c r="F76" t="s">
-        <v>11</v>
-      </c>
-      <c r="G76" t="s">
-        <v>15</v>
-      </c>
-      <c r="H76" t="s">
-        <v>192</v>
       </c>
       <c r="I76" t="s">
         <v>11</v>
@@ -4003,7 +4000,7 @@
         <v>11</v>
       </c>
       <c r="L76" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -4014,7 +4011,7 @@
         <v>2</v>
       </c>
       <c r="C77" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D77" t="s">
         <v>11</v>
@@ -4029,7 +4026,7 @@
         <v>11</v>
       </c>
       <c r="H77" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I77" t="s">
         <v>11</v>
@@ -4041,7 +4038,7 @@
         <v>15</v>
       </c>
       <c r="L77" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -4079,7 +4076,7 @@
         <v>11</v>
       </c>
       <c r="L78" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -4090,22 +4087,22 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
+        <v>105</v>
+      </c>
+      <c r="D79" t="s">
+        <v>15</v>
+      </c>
+      <c r="E79" t="s">
+        <v>15</v>
+      </c>
+      <c r="F79" t="s">
+        <v>11</v>
+      </c>
+      <c r="G79" t="s">
+        <v>15</v>
+      </c>
+      <c r="H79" t="s">
         <v>106</v>
-      </c>
-      <c r="D79" t="s">
-        <v>15</v>
-      </c>
-      <c r="E79" t="s">
-        <v>15</v>
-      </c>
-      <c r="F79" t="s">
-        <v>11</v>
-      </c>
-      <c r="G79" t="s">
-        <v>15</v>
-      </c>
-      <c r="H79" t="s">
-        <v>107</v>
       </c>
       <c r="I79" t="s">
         <v>11</v>
@@ -4117,7 +4114,7 @@
         <v>11</v>
       </c>
       <c r="L79" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
@@ -4143,7 +4140,7 @@
         <v>15</v>
       </c>
       <c r="H80" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I80" t="s">
         <v>11</v>
@@ -4155,7 +4152,7 @@
         <v>11</v>
       </c>
       <c r="L80" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -4166,7 +4163,7 @@
         <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D81" t="s">
         <v>15</v>
@@ -4181,7 +4178,7 @@
         <v>15</v>
       </c>
       <c r="H81" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I81" t="s">
         <v>11</v>
@@ -4193,7 +4190,7 @@
         <v>11</v>
       </c>
       <c r="L81" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -4204,7 +4201,7 @@
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D82" t="s">
         <v>11</v>
@@ -4219,7 +4216,7 @@
         <v>11</v>
       </c>
       <c r="H82" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I82" t="s">
         <v>11</v>
@@ -4231,7 +4228,7 @@
         <v>11</v>
       </c>
       <c r="L82" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -4242,7 +4239,7 @@
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D83" t="s">
         <v>11</v>
@@ -4257,19 +4254,19 @@
         <v>11</v>
       </c>
       <c r="H83" t="s">
+        <v>201</v>
+      </c>
+      <c r="I83" t="s">
+        <v>11</v>
+      </c>
+      <c r="J83" t="s">
+        <v>176</v>
+      </c>
+      <c r="K83" t="s">
+        <v>11</v>
+      </c>
+      <c r="L83" t="s">
         <v>202</v>
-      </c>
-      <c r="I83" t="s">
-        <v>11</v>
-      </c>
-      <c r="J83" t="s">
-        <v>177</v>
-      </c>
-      <c r="K83" t="s">
-        <v>11</v>
-      </c>
-      <c r="L83" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -4280,7 +4277,7 @@
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D84" t="s">
         <v>11</v>
@@ -4295,7 +4292,7 @@
         <v>11</v>
       </c>
       <c r="H84" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I84" t="s">
         <v>11</v>
@@ -4307,7 +4304,7 @@
         <v>11</v>
       </c>
       <c r="L84" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -4318,7 +4315,7 @@
         <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D85" t="s">
         <v>60</v>
@@ -4345,7 +4342,7 @@
         <v>11</v>
       </c>
       <c r="L85" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -4356,7 +4353,7 @@
         <v>2</v>
       </c>
       <c r="C86" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D86" t="s">
         <v>11</v>
@@ -4371,7 +4368,7 @@
         <v>15</v>
       </c>
       <c r="H86" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I86" t="s">
         <v>11</v>
@@ -4383,7 +4380,7 @@
         <v>11</v>
       </c>
       <c r="L86" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
@@ -4394,7 +4391,7 @@
         <v>1</v>
       </c>
       <c r="C87" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D87" t="s">
         <v>11</v>
@@ -4409,7 +4406,7 @@
         <v>11</v>
       </c>
       <c r="H87" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I87" t="s">
         <v>11</v>
@@ -4421,7 +4418,7 @@
         <v>15</v>
       </c>
       <c r="L87" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
@@ -4447,7 +4444,7 @@
         <v>15</v>
       </c>
       <c r="H88" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I88" t="s">
         <v>11</v>
@@ -4459,7 +4456,7 @@
         <v>11</v>
       </c>
       <c r="L88" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
@@ -4470,7 +4467,7 @@
         <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D89" t="s">
         <v>11</v>
@@ -4485,7 +4482,7 @@
         <v>15</v>
       </c>
       <c r="H89" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I89" t="s">
         <v>11</v>
@@ -4497,7 +4494,7 @@
         <v>11</v>
       </c>
       <c r="L89" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
@@ -4523,7 +4520,7 @@
         <v>15</v>
       </c>
       <c r="H90" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I90" t="s">
         <v>11</v>
@@ -4535,7 +4532,7 @@
         <v>11</v>
       </c>
       <c r="L90" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -4546,7 +4543,7 @@
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D91" t="s">
         <v>11</v>
@@ -4561,7 +4558,7 @@
         <v>11</v>
       </c>
       <c r="H91" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I91" t="s">
         <v>11</v>
@@ -4573,7 +4570,7 @@
         <v>11</v>
       </c>
       <c r="L91" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -4584,7 +4581,7 @@
         <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D92" t="s">
         <v>15</v>
@@ -4599,7 +4596,7 @@
         <v>15</v>
       </c>
       <c r="H92" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I92" t="s">
         <v>11</v>
@@ -4611,7 +4608,7 @@
         <v>11</v>
       </c>
       <c r="L92" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -4622,7 +4619,7 @@
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D93" t="s">
         <v>11</v>
@@ -4637,7 +4634,7 @@
         <v>15</v>
       </c>
       <c r="H93" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I93" t="s">
         <v>11</v>
@@ -4649,7 +4646,7 @@
         <v>11</v>
       </c>
       <c r="L93" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -4660,7 +4657,7 @@
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D94" t="s">
         <v>15</v>
@@ -4675,7 +4672,7 @@
         <v>15</v>
       </c>
       <c r="H94" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I94" t="s">
         <v>11</v>
@@ -4687,7 +4684,7 @@
         <v>11</v>
       </c>
       <c r="L94" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -4698,7 +4695,7 @@
         <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D95" t="s">
         <v>11</v>
@@ -4713,7 +4710,7 @@
         <v>11</v>
       </c>
       <c r="H95" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I95" t="s">
         <v>11</v>
@@ -4725,7 +4722,7 @@
         <v>11</v>
       </c>
       <c r="L95" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -4771,10 +4768,10 @@
         <v>95</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D97" t="s">
         <v>15</v>
@@ -4789,7 +4786,7 @@
         <v>15</v>
       </c>
       <c r="H97" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I97" t="s">
         <v>11</v>
@@ -4801,7 +4798,7 @@
         <v>11</v>
       </c>
       <c r="L97" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -4809,10 +4806,10 @@
         <v>96</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C98" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D98" t="s">
         <v>15</v>
@@ -4827,7 +4824,7 @@
         <v>15</v>
       </c>
       <c r="H98" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I98" t="s">
         <v>11</v>
@@ -4839,7 +4836,7 @@
         <v>11</v>
       </c>
       <c r="L98" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -4850,7 +4847,7 @@
         <v>2</v>
       </c>
       <c r="C99" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D99" t="s">
         <v>11</v>
@@ -4865,19 +4862,19 @@
         <v>15</v>
       </c>
       <c r="H99" t="s">
+        <v>229</v>
+      </c>
+      <c r="I99" t="s">
+        <v>11</v>
+      </c>
+      <c r="J99" t="s">
         <v>230</v>
       </c>
-      <c r="I99" t="s">
-        <v>11</v>
-      </c>
-      <c r="J99" t="s">
+      <c r="K99" t="s">
+        <v>11</v>
+      </c>
+      <c r="L99" t="s">
         <v>231</v>
-      </c>
-      <c r="K99" t="s">
-        <v>11</v>
-      </c>
-      <c r="L99" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -4888,7 +4885,7 @@
         <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D100" t="s">
         <v>60</v>
@@ -4903,19 +4900,19 @@
         <v>15</v>
       </c>
       <c r="H100" t="s">
+        <v>232</v>
+      </c>
+      <c r="I100" t="s">
+        <v>11</v>
+      </c>
+      <c r="J100" t="s">
         <v>233</v>
       </c>
-      <c r="I100" t="s">
-        <v>11</v>
-      </c>
-      <c r="J100" t="s">
+      <c r="K100" t="s">
+        <v>11</v>
+      </c>
+      <c r="L100" t="s">
         <v>234</v>
-      </c>
-      <c r="K100" t="s">
-        <v>11</v>
-      </c>
-      <c r="L100" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -4926,7 +4923,7 @@
         <v>2</v>
       </c>
       <c r="C101" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D101" t="s">
         <v>11</v>
@@ -4941,7 +4938,7 @@
         <v>15</v>
       </c>
       <c r="H101" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I101" t="s">
         <v>11</v>
@@ -4953,7 +4950,7 @@
         <v>11</v>
       </c>
       <c r="L101" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
@@ -4964,7 +4961,7 @@
         <v>2</v>
       </c>
       <c r="C102" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D102" t="s">
         <v>11</v>
@@ -4979,19 +4976,19 @@
         <v>15</v>
       </c>
       <c r="H102" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I102" t="s">
         <v>11</v>
       </c>
       <c r="J102" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K102" t="s">
         <v>11</v>
       </c>
       <c r="L102" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
@@ -5002,7 +4999,7 @@
         <v>2</v>
       </c>
       <c r="C103" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D103" t="s">
         <v>15</v>
@@ -5017,19 +5014,19 @@
         <v>15</v>
       </c>
       <c r="H103" t="s">
+        <v>238</v>
+      </c>
+      <c r="I103" t="s">
+        <v>11</v>
+      </c>
+      <c r="J103" t="s">
+        <v>157</v>
+      </c>
+      <c r="K103" t="s">
+        <v>11</v>
+      </c>
+      <c r="L103" t="s">
         <v>239</v>
-      </c>
-      <c r="I103" t="s">
-        <v>11</v>
-      </c>
-      <c r="J103" t="s">
-        <v>158</v>
-      </c>
-      <c r="K103" t="s">
-        <v>11</v>
-      </c>
-      <c r="L103" t="s">
-        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
times for every step -- not finished combine images
</commit_message>
<xml_diff>
--- a/accident_ground_truths.xlsx
+++ b/accident_ground_truths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B06FBF-ED89-49FE-81A0-32BAE67F45D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD889CB-9DFA-4C63-A98F-43E968EB501B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="254">
   <si>
     <t>Number of vehicles in accident</t>
   </si>
@@ -740,6 +740,48 @@
   </si>
   <si>
     <t>big vehicle looks to have run a red light and, as a result, the biker hits the vehicle</t>
+  </si>
+  <si>
+    <t>angled t-bone</t>
+  </si>
+  <si>
+    <t>Cloudy</t>
+  </si>
+  <si>
+    <t>super busy intersection</t>
+  </si>
+  <si>
+    <t>extremely difficult to see</t>
+  </si>
+  <si>
+    <t>bike runs into suv, only biker seems injured</t>
+  </si>
+  <si>
+    <t>Truck runs into bike</t>
+  </si>
+  <si>
+    <t>sedan x2, bus</t>
+  </si>
+  <si>
+    <t>Bus runs into sedan which runs into other sedan</t>
+  </si>
+  <si>
+    <t>loss of control</t>
+  </si>
+  <si>
+    <t>sedan</t>
+  </si>
+  <si>
+    <t>car runs into median in city</t>
+  </si>
+  <si>
+    <t>sedan runs into bus at non-busy intersection</t>
+  </si>
+  <si>
+    <t>Bike topples over, injury seems minor, unknown if any other vehicle was involved</t>
+  </si>
+  <si>
+    <t>The glare makes it difficult to tell what exactly happened</t>
   </si>
 </sst>
 </file>
@@ -1104,10 +1146,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K77" sqref="K77"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5029,6 +5071,386 @@
         <v>239</v>
       </c>
     </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="3">
+        <v>102</v>
+      </c>
+      <c r="B104" s="3">
+        <v>2</v>
+      </c>
+      <c r="C104" t="s">
+        <v>240</v>
+      </c>
+      <c r="D104" t="s">
+        <v>15</v>
+      </c>
+      <c r="E104" t="s">
+        <v>15</v>
+      </c>
+      <c r="F104" t="s">
+        <v>11</v>
+      </c>
+      <c r="G104" t="s">
+        <v>15</v>
+      </c>
+      <c r="H104" t="s">
+        <v>211</v>
+      </c>
+      <c r="I104" t="s">
+        <v>11</v>
+      </c>
+      <c r="J104" t="s">
+        <v>241</v>
+      </c>
+      <c r="K104" t="s">
+        <v>11</v>
+      </c>
+      <c r="L104" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A105" s="3">
+        <v>103</v>
+      </c>
+      <c r="B105" s="3">
+        <v>2</v>
+      </c>
+      <c r="C105" t="s">
+        <v>163</v>
+      </c>
+      <c r="D105" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105" t="s">
+        <v>11</v>
+      </c>
+      <c r="F105" t="s">
+        <v>11</v>
+      </c>
+      <c r="G105" t="s">
+        <v>11</v>
+      </c>
+      <c r="H105" t="s">
+        <v>46</v>
+      </c>
+      <c r="I105" t="s">
+        <v>11</v>
+      </c>
+      <c r="J105" t="s">
+        <v>37</v>
+      </c>
+      <c r="K105" t="s">
+        <v>11</v>
+      </c>
+      <c r="L105" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A106" s="3">
+        <v>104</v>
+      </c>
+      <c r="B106" s="3">
+        <v>2</v>
+      </c>
+      <c r="C106" t="s">
+        <v>240</v>
+      </c>
+      <c r="D106" t="s">
+        <v>15</v>
+      </c>
+      <c r="E106" t="s">
+        <v>15</v>
+      </c>
+      <c r="F106" t="s">
+        <v>11</v>
+      </c>
+      <c r="G106" t="s">
+        <v>15</v>
+      </c>
+      <c r="H106" t="s">
+        <v>61</v>
+      </c>
+      <c r="I106" t="s">
+        <v>11</v>
+      </c>
+      <c r="J106" t="s">
+        <v>26</v>
+      </c>
+      <c r="K106" t="s">
+        <v>15</v>
+      </c>
+      <c r="L106" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107" s="3">
+        <v>105</v>
+      </c>
+      <c r="B107" s="3">
+        <v>2</v>
+      </c>
+      <c r="C107" t="s">
+        <v>100</v>
+      </c>
+      <c r="D107" t="s">
+        <v>15</v>
+      </c>
+      <c r="E107" t="s">
+        <v>15</v>
+      </c>
+      <c r="F107" t="s">
+        <v>11</v>
+      </c>
+      <c r="G107" t="s">
+        <v>15</v>
+      </c>
+      <c r="H107" t="s">
+        <v>232</v>
+      </c>
+      <c r="I107" t="s">
+        <v>11</v>
+      </c>
+      <c r="J107" t="s">
+        <v>43</v>
+      </c>
+      <c r="K107" t="s">
+        <v>11</v>
+      </c>
+      <c r="L107" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A108" s="3">
+        <v>106</v>
+      </c>
+      <c r="B108" s="3">
+        <v>2</v>
+      </c>
+      <c r="C108" t="s">
+        <v>100</v>
+      </c>
+      <c r="D108" t="s">
+        <v>15</v>
+      </c>
+      <c r="E108" t="s">
+        <v>15</v>
+      </c>
+      <c r="F108" t="s">
+        <v>11</v>
+      </c>
+      <c r="G108" t="s">
+        <v>15</v>
+      </c>
+      <c r="H108" t="s">
+        <v>224</v>
+      </c>
+      <c r="I108" t="s">
+        <v>11</v>
+      </c>
+      <c r="J108" t="s">
+        <v>43</v>
+      </c>
+      <c r="K108" t="s">
+        <v>11</v>
+      </c>
+      <c r="L108" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A109" s="3">
+        <v>107</v>
+      </c>
+      <c r="B109" s="3">
+        <v>3</v>
+      </c>
+      <c r="C109" t="s">
+        <v>163</v>
+      </c>
+      <c r="D109" t="s">
+        <v>15</v>
+      </c>
+      <c r="E109" t="s">
+        <v>15</v>
+      </c>
+      <c r="F109" t="s">
+        <v>11</v>
+      </c>
+      <c r="G109" t="s">
+        <v>15</v>
+      </c>
+      <c r="H109" t="s">
+        <v>246</v>
+      </c>
+      <c r="I109" t="s">
+        <v>11</v>
+      </c>
+      <c r="J109" t="s">
+        <v>43</v>
+      </c>
+      <c r="K109" t="s">
+        <v>11</v>
+      </c>
+      <c r="L109" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A110" s="3">
+        <v>108</v>
+      </c>
+      <c r="B110" s="3">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>248</v>
+      </c>
+      <c r="D110" t="s">
+        <v>15</v>
+      </c>
+      <c r="E110" t="s">
+        <v>15</v>
+      </c>
+      <c r="F110" t="s">
+        <v>11</v>
+      </c>
+      <c r="G110" t="s">
+        <v>15</v>
+      </c>
+      <c r="H110" t="s">
+        <v>249</v>
+      </c>
+      <c r="I110" t="s">
+        <v>11</v>
+      </c>
+      <c r="J110" t="s">
+        <v>43</v>
+      </c>
+      <c r="K110" t="s">
+        <v>11</v>
+      </c>
+      <c r="L110" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A111" s="3">
+        <v>109</v>
+      </c>
+      <c r="B111" s="3">
+        <v>2</v>
+      </c>
+      <c r="C111" t="s">
+        <v>100</v>
+      </c>
+      <c r="D111" t="s">
+        <v>15</v>
+      </c>
+      <c r="E111" t="s">
+        <v>15</v>
+      </c>
+      <c r="F111" t="s">
+        <v>11</v>
+      </c>
+      <c r="G111" t="s">
+        <v>15</v>
+      </c>
+      <c r="H111" t="s">
+        <v>85</v>
+      </c>
+      <c r="I111" t="s">
+        <v>11</v>
+      </c>
+      <c r="J111" t="s">
+        <v>26</v>
+      </c>
+      <c r="K111" t="s">
+        <v>11</v>
+      </c>
+      <c r="L111" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A112" s="3">
+        <v>110</v>
+      </c>
+      <c r="B112" s="3">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>105</v>
+      </c>
+      <c r="D112" t="s">
+        <v>15</v>
+      </c>
+      <c r="E112" t="s">
+        <v>15</v>
+      </c>
+      <c r="F112" t="s">
+        <v>11</v>
+      </c>
+      <c r="G112" t="s">
+        <v>15</v>
+      </c>
+      <c r="H112" t="s">
+        <v>201</v>
+      </c>
+      <c r="I112" t="s">
+        <v>11</v>
+      </c>
+      <c r="J112" t="s">
+        <v>43</v>
+      </c>
+      <c r="K112" t="s">
+        <v>11</v>
+      </c>
+      <c r="L112" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A113" s="3">
+        <v>111</v>
+      </c>
+      <c r="B113" s="3">
+        <v>2</v>
+      </c>
+      <c r="C113" t="s">
+        <v>100</v>
+      </c>
+      <c r="D113" t="s">
+        <v>15</v>
+      </c>
+      <c r="E113" t="s">
+        <v>15</v>
+      </c>
+      <c r="F113" t="s">
+        <v>11</v>
+      </c>
+      <c r="G113" t="s">
+        <v>15</v>
+      </c>
+      <c r="H113" t="s">
+        <v>166</v>
+      </c>
+      <c r="I113" t="s">
+        <v>11</v>
+      </c>
+      <c r="J113" t="s">
+        <v>26</v>
+      </c>
+      <c r="K113" t="s">
+        <v>15</v>
+      </c>
+      <c r="L113" t="s">
+        <v>253</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed json comma issue
</commit_message>
<xml_diff>
--- a/accident_ground_truths.xlsx
+++ b/accident_ground_truths.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD889CB-9DFA-4C63-A98F-43E968EB501B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D3F76B-EF3B-4FC4-AA39-36875A3E5787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="266">
   <si>
     <t>Number of vehicles in accident</t>
   </si>
@@ -782,6 +782,42 @@
   </si>
   <si>
     <t>The glare makes it difficult to tell what exactly happened</t>
+  </si>
+  <si>
+    <t>Fender Bender</t>
+  </si>
+  <si>
+    <t>slight t-bone</t>
+  </si>
+  <si>
+    <t>Roundabout</t>
+  </si>
+  <si>
+    <t>intersection</t>
+  </si>
+  <si>
+    <t>motorbike, suv</t>
+  </si>
+  <si>
+    <t>Motorcyclist runs into suv and falls off</t>
+  </si>
+  <si>
+    <t>intsection at a light</t>
+  </si>
+  <si>
+    <t>intersection/roundabout</t>
+  </si>
+  <si>
+    <t>light side-on-side collision</t>
+  </si>
+  <si>
+    <t>hit car spins out</t>
+  </si>
+  <si>
+    <t>front-end collision</t>
+  </si>
+  <si>
+    <t>tuck hits and topples bike</t>
   </si>
 </sst>
 </file>
@@ -1146,10 +1182,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L113"/>
+  <dimension ref="A1:L127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128:A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5451,6 +5487,538 @@
         <v>253</v>
       </c>
     </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A114" s="3">
+        <v>112</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114" t="s">
+        <v>10</v>
+      </c>
+      <c r="D114" t="s">
+        <v>11</v>
+      </c>
+      <c r="E114" t="s">
+        <v>11</v>
+      </c>
+      <c r="F114" t="s">
+        <v>11</v>
+      </c>
+      <c r="G114" t="s">
+        <v>11</v>
+      </c>
+      <c r="H114" t="s">
+        <v>10</v>
+      </c>
+      <c r="I114" t="s">
+        <v>11</v>
+      </c>
+      <c r="J114" t="s">
+        <v>43</v>
+      </c>
+      <c r="K114" t="s">
+        <v>11</v>
+      </c>
+      <c r="L114" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A115" s="3">
+        <v>113</v>
+      </c>
+      <c r="B115" s="3">
+        <v>2</v>
+      </c>
+      <c r="C115" t="s">
+        <v>163</v>
+      </c>
+      <c r="D115" t="s">
+        <v>11</v>
+      </c>
+      <c r="E115" t="s">
+        <v>11</v>
+      </c>
+      <c r="F115" t="s">
+        <v>11</v>
+      </c>
+      <c r="G115" t="s">
+        <v>11</v>
+      </c>
+      <c r="H115" t="s">
+        <v>24</v>
+      </c>
+      <c r="I115" t="s">
+        <v>11</v>
+      </c>
+      <c r="J115" t="s">
+        <v>26</v>
+      </c>
+      <c r="K115" t="s">
+        <v>11</v>
+      </c>
+      <c r="L115" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A116" s="3">
+        <v>114</v>
+      </c>
+      <c r="B116" s="3">
+        <v>2</v>
+      </c>
+      <c r="C116" t="s">
+        <v>163</v>
+      </c>
+      <c r="D116" t="s">
+        <v>11</v>
+      </c>
+      <c r="E116" t="s">
+        <v>11</v>
+      </c>
+      <c r="F116" t="s">
+        <v>11</v>
+      </c>
+      <c r="G116" t="s">
+        <v>11</v>
+      </c>
+      <c r="H116" t="s">
+        <v>24</v>
+      </c>
+      <c r="I116" t="s">
+        <v>11</v>
+      </c>
+      <c r="J116" t="s">
+        <v>26</v>
+      </c>
+      <c r="K116" t="s">
+        <v>11</v>
+      </c>
+      <c r="L116" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A117" s="3">
+        <v>115</v>
+      </c>
+      <c r="B117" s="3">
+        <v>2</v>
+      </c>
+      <c r="C117" t="s">
+        <v>255</v>
+      </c>
+      <c r="D117" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117" t="s">
+        <v>11</v>
+      </c>
+      <c r="F117" t="s">
+        <v>11</v>
+      </c>
+      <c r="G117" t="s">
+        <v>15</v>
+      </c>
+      <c r="H117" t="s">
+        <v>164</v>
+      </c>
+      <c r="I117" t="s">
+        <v>11</v>
+      </c>
+      <c r="J117" t="s">
+        <v>43</v>
+      </c>
+      <c r="K117" t="s">
+        <v>11</v>
+      </c>
+      <c r="L117" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118" s="3">
+        <v>116</v>
+      </c>
+      <c r="B118" s="3">
+        <v>2</v>
+      </c>
+      <c r="C118" t="s">
+        <v>100</v>
+      </c>
+      <c r="D118" t="s">
+        <v>15</v>
+      </c>
+      <c r="E118" t="s">
+        <v>15</v>
+      </c>
+      <c r="F118" t="s">
+        <v>11</v>
+      </c>
+      <c r="G118" t="s">
+        <v>15</v>
+      </c>
+      <c r="H118" t="s">
+        <v>166</v>
+      </c>
+      <c r="I118" t="s">
+        <v>11</v>
+      </c>
+      <c r="J118" t="s">
+        <v>43</v>
+      </c>
+      <c r="K118" t="s">
+        <v>11</v>
+      </c>
+      <c r="L118" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A119" s="3">
+        <v>117</v>
+      </c>
+      <c r="B119" s="3">
+        <v>2</v>
+      </c>
+      <c r="C119" t="s">
+        <v>255</v>
+      </c>
+      <c r="D119" t="s">
+        <v>11</v>
+      </c>
+      <c r="E119" t="s">
+        <v>11</v>
+      </c>
+      <c r="F119" t="s">
+        <v>11</v>
+      </c>
+      <c r="G119" t="s">
+        <v>15</v>
+      </c>
+      <c r="H119" t="s">
+        <v>46</v>
+      </c>
+      <c r="I119" t="s">
+        <v>11</v>
+      </c>
+      <c r="J119" t="s">
+        <v>43</v>
+      </c>
+      <c r="K119" t="s">
+        <v>11</v>
+      </c>
+      <c r="L119" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A120" s="3">
+        <v>118</v>
+      </c>
+      <c r="B120" s="3">
+        <v>2</v>
+      </c>
+      <c r="C120" t="s">
+        <v>163</v>
+      </c>
+      <c r="D120" t="s">
+        <v>15</v>
+      </c>
+      <c r="E120" t="s">
+        <v>15</v>
+      </c>
+      <c r="F120" t="s">
+        <v>11</v>
+      </c>
+      <c r="G120" t="s">
+        <v>15</v>
+      </c>
+      <c r="H120" t="s">
+        <v>258</v>
+      </c>
+      <c r="I120" t="s">
+        <v>11</v>
+      </c>
+      <c r="J120" t="s">
+        <v>43</v>
+      </c>
+      <c r="K120" t="s">
+        <v>11</v>
+      </c>
+      <c r="L120" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A121" s="3">
+        <v>119</v>
+      </c>
+      <c r="B121" s="3">
+        <v>2</v>
+      </c>
+      <c r="C121" t="s">
+        <v>100</v>
+      </c>
+      <c r="D121" t="s">
+        <v>15</v>
+      </c>
+      <c r="E121" t="s">
+        <v>15</v>
+      </c>
+      <c r="F121" t="s">
+        <v>11</v>
+      </c>
+      <c r="G121" t="s">
+        <v>15</v>
+      </c>
+      <c r="H121" t="s">
+        <v>46</v>
+      </c>
+      <c r="I121" t="s">
+        <v>11</v>
+      </c>
+      <c r="J121" t="s">
+        <v>230</v>
+      </c>
+      <c r="K121" t="s">
+        <v>11</v>
+      </c>
+      <c r="L121" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A122" s="3">
+        <v>120</v>
+      </c>
+      <c r="B122" s="3">
+        <v>2</v>
+      </c>
+      <c r="C122" t="s">
+        <v>100</v>
+      </c>
+      <c r="D122" t="s">
+        <v>15</v>
+      </c>
+      <c r="E122" t="s">
+        <v>15</v>
+      </c>
+      <c r="F122" t="s">
+        <v>11</v>
+      </c>
+      <c r="G122" t="s">
+        <v>15</v>
+      </c>
+      <c r="H122" t="s">
+        <v>166</v>
+      </c>
+      <c r="I122" t="s">
+        <v>11</v>
+      </c>
+      <c r="J122" t="s">
+        <v>230</v>
+      </c>
+      <c r="K122" t="s">
+        <v>11</v>
+      </c>
+      <c r="L122" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A123" s="3">
+        <v>121</v>
+      </c>
+      <c r="B123" s="3">
+        <v>2</v>
+      </c>
+      <c r="C123" t="s">
+        <v>100</v>
+      </c>
+      <c r="D123" t="s">
+        <v>15</v>
+      </c>
+      <c r="E123" t="s">
+        <v>15</v>
+      </c>
+      <c r="F123" t="s">
+        <v>11</v>
+      </c>
+      <c r="G123" t="s">
+        <v>15</v>
+      </c>
+      <c r="H123" t="s">
+        <v>61</v>
+      </c>
+      <c r="I123" t="s">
+        <v>11</v>
+      </c>
+      <c r="J123" t="s">
+        <v>37</v>
+      </c>
+      <c r="K123" t="s">
+        <v>11</v>
+      </c>
+      <c r="L123" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A124" s="3">
+        <v>122</v>
+      </c>
+      <c r="B124" s="3">
+        <v>2</v>
+      </c>
+      <c r="C124" t="s">
+        <v>100</v>
+      </c>
+      <c r="D124" t="s">
+        <v>15</v>
+      </c>
+      <c r="E124" t="s">
+        <v>15</v>
+      </c>
+      <c r="F124" t="s">
+        <v>11</v>
+      </c>
+      <c r="G124" t="s">
+        <v>15</v>
+      </c>
+      <c r="H124" t="s">
+        <v>46</v>
+      </c>
+      <c r="I124" t="s">
+        <v>11</v>
+      </c>
+      <c r="J124" t="s">
+        <v>26</v>
+      </c>
+      <c r="K124" t="s">
+        <v>15</v>
+      </c>
+      <c r="L124" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A125" s="3">
+        <v>123</v>
+      </c>
+      <c r="B125" s="3">
+        <v>2</v>
+      </c>
+      <c r="C125" t="s">
+        <v>262</v>
+      </c>
+      <c r="D125" t="s">
+        <v>11</v>
+      </c>
+      <c r="E125" t="s">
+        <v>11</v>
+      </c>
+      <c r="F125" t="s">
+        <v>11</v>
+      </c>
+      <c r="G125" t="s">
+        <v>15</v>
+      </c>
+      <c r="H125" t="s">
+        <v>85</v>
+      </c>
+      <c r="I125" t="s">
+        <v>11</v>
+      </c>
+      <c r="J125" t="s">
+        <v>43</v>
+      </c>
+      <c r="K125" t="s">
+        <v>11</v>
+      </c>
+      <c r="L125" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A126" s="3">
+        <v>124</v>
+      </c>
+      <c r="B126" s="3">
+        <v>2</v>
+      </c>
+      <c r="C126" t="s">
+        <v>100</v>
+      </c>
+      <c r="D126" t="s">
+        <v>15</v>
+      </c>
+      <c r="E126" t="s">
+        <v>15</v>
+      </c>
+      <c r="F126" t="s">
+        <v>11</v>
+      </c>
+      <c r="G126" t="s">
+        <v>15</v>
+      </c>
+      <c r="H126" t="s">
+        <v>137</v>
+      </c>
+      <c r="I126" t="s">
+        <v>11</v>
+      </c>
+      <c r="J126" t="s">
+        <v>54</v>
+      </c>
+      <c r="K126" t="s">
+        <v>11</v>
+      </c>
+      <c r="L126" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A127" s="3">
+        <v>125</v>
+      </c>
+      <c r="B127" s="3">
+        <v>2</v>
+      </c>
+      <c r="C127" t="s">
+        <v>264</v>
+      </c>
+      <c r="D127" t="s">
+        <v>15</v>
+      </c>
+      <c r="E127" t="s">
+        <v>15</v>
+      </c>
+      <c r="F127" t="s">
+        <v>11</v>
+      </c>
+      <c r="G127" t="s">
+        <v>15</v>
+      </c>
+      <c r="H127" t="s">
+        <v>124</v>
+      </c>
+      <c r="I127" t="s">
+        <v>11</v>
+      </c>
+      <c r="J127" t="s">
+        <v>54</v>
+      </c>
+      <c r="K127" t="s">
+        <v>11</v>
+      </c>
+      <c r="L127" t="s">
+        <v>265</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ground truths for 200 samples
</commit_message>
<xml_diff>
--- a/accident_ground_truths.xlsx
+++ b/accident_ground_truths.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D3F76B-EF3B-4FC4-AA39-36875A3E5787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8074D44E-5068-471D-9DE5-2AEE455E37B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="339">
   <si>
     <t>Number of vehicles in accident</t>
   </si>
@@ -817,14 +830,233 @@
     <t>front-end collision</t>
   </si>
   <si>
-    <t>tuck hits and topples bike</t>
+    <t>rear-end collision</t>
+  </si>
+  <si>
+    <t>truck hits and topples bike</t>
+  </si>
+  <si>
+    <t>near intersection</t>
+  </si>
+  <si>
+    <t>little/no traffic</t>
+  </si>
+  <si>
+    <t>lots of traffic</t>
+  </si>
+  <si>
+    <t>truck,sedan</t>
+  </si>
+  <si>
+    <t>sedan x3</t>
+  </si>
+  <si>
+    <t>sedan hits other sedan into bus on intersection</t>
+  </si>
+  <si>
+    <t>intersection, light traffic</t>
+  </si>
+  <si>
+    <t>spin out into front-end collision</t>
+  </si>
+  <si>
+    <t>suv x2, bike x2, bus</t>
+  </si>
+  <si>
+    <t>main collision is with the two vehicles, the other three got caught in the crossfire. Damage is great</t>
+  </si>
+  <si>
+    <t>no accident occurred</t>
+  </si>
+  <si>
+    <t>intersection with traffic</t>
+  </si>
+  <si>
+    <t>spin-out into light t-bone</t>
+  </si>
+  <si>
+    <t>driver lost control and tapped other driver</t>
+  </si>
+  <si>
+    <t>front-end collision into object</t>
+  </si>
+  <si>
+    <t>driver loses control and hits a pole</t>
+  </si>
+  <si>
+    <t>little traffic</t>
+  </si>
+  <si>
+    <t>Night, clear</t>
+  </si>
+  <si>
+    <t>intersection, driver ran a red light</t>
+  </si>
+  <si>
+    <t>pedestrian collision</t>
+  </si>
+  <si>
+    <t>suv hits two pedestrians lightly</t>
+  </si>
+  <si>
+    <t>light pedestrian collision</t>
+  </si>
+  <si>
+    <t>truck hits two pedestrians and hits a tree</t>
+  </si>
+  <si>
+    <t>SUV hits truck</t>
+  </si>
+  <si>
+    <t>top collision</t>
+  </si>
+  <si>
+    <t>commercial truck</t>
+  </si>
+  <si>
+    <t>Commercial truck does not make clearance</t>
+  </si>
+  <si>
+    <t>dump truck, sedan x4, van</t>
+  </si>
+  <si>
+    <t>Dump truck topples over and damages adjacent vehicles. Damage is high</t>
+  </si>
+  <si>
+    <t>9+</t>
+  </si>
+  <si>
+    <t>sedans, suvs, truck</t>
+  </si>
+  <si>
+    <t>Unknown what happened, poor road conditions</t>
+  </si>
+  <si>
+    <t>possibly a small collision, but hard to tell from footage</t>
+  </si>
+  <si>
+    <t>backs into pedestrian</t>
+  </si>
+  <si>
+    <t>No damage occurs, no traffic</t>
+  </si>
+  <si>
+    <t>probably slippery</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>big vehicle hits person</t>
+  </si>
+  <si>
+    <t>motorbike, sedan</t>
+  </si>
+  <si>
+    <t>intersection, medium traffic</t>
+  </si>
+  <si>
+    <t>interstate or highway</t>
+  </si>
+  <si>
+    <t>Intersection</t>
+  </si>
+  <si>
+    <t>highway or interstate</t>
+  </si>
+  <si>
+    <t>sedan x4</t>
+  </si>
+  <si>
+    <t>initial collision into other collisions</t>
+  </si>
+  <si>
+    <t>pedestrian seems extremely hurt</t>
+  </si>
+  <si>
+    <t>no injuries seen</t>
+  </si>
+  <si>
+    <t>van, truck</t>
+  </si>
+  <si>
+    <t>suv x2, bike</t>
+  </si>
+  <si>
+    <t>medium traffic</t>
+  </si>
+  <si>
+    <t>intersection, no traffic</t>
+  </si>
+  <si>
+    <t>intersection, heavy traffic</t>
+  </si>
+  <si>
+    <t>intersection with light</t>
+  </si>
+  <si>
+    <t>intersection with light, heavy traffic</t>
+  </si>
+  <si>
+    <t>interseciton</t>
+  </si>
+  <si>
+    <t>person injury level probably severe</t>
+  </si>
+  <si>
+    <t>truck, 18-wheeler</t>
+  </si>
+  <si>
+    <t>damage high</t>
+  </si>
+  <si>
+    <t>18-wheeler x2</t>
+  </si>
+  <si>
+    <t>low damage</t>
+  </si>
+  <si>
+    <t>object collision</t>
+  </si>
+  <si>
+    <t>car hits sign</t>
+  </si>
+  <si>
+    <t>bus , sedan x2</t>
+  </si>
+  <si>
+    <t>cars hit bus that spun out</t>
+  </si>
+  <si>
+    <t>bike, bus</t>
+  </si>
+  <si>
+    <t>bike hits pedestrian who then gets hit by bus</t>
+  </si>
+  <si>
+    <t>bike x2</t>
+  </si>
+  <si>
+    <t>little to no injury and damage</t>
+  </si>
+  <si>
+    <t>van, bike</t>
+  </si>
+  <si>
+    <t>bike, van</t>
+  </si>
+  <si>
+    <t>little to no injury or damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sedan, bike </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -837,6 +1069,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1182,10 +1420,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L127"/>
+  <dimension ref="A1:L202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128:A134"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="B203" sqref="B203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6016,10 +6254,2861 @@
         <v>11</v>
       </c>
       <c r="L127" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A128" s="3">
+        <v>126</v>
+      </c>
+      <c r="B128" s="3">
+        <v>2</v>
+      </c>
+      <c r="C128" t="s">
         <v>265</v>
       </c>
+      <c r="D128" t="s">
+        <v>15</v>
+      </c>
+      <c r="E128" t="s">
+        <v>15</v>
+      </c>
+      <c r="F128" t="s">
+        <v>11</v>
+      </c>
+      <c r="G128" t="s">
+        <v>15</v>
+      </c>
+      <c r="H128" t="s">
+        <v>197</v>
+      </c>
+      <c r="I128" t="s">
+        <v>11</v>
+      </c>
+      <c r="J128" t="s">
+        <v>54</v>
+      </c>
+      <c r="K128" t="s">
+        <v>11</v>
+      </c>
+      <c r="L128" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A129" s="3">
+        <v>127</v>
+      </c>
+      <c r="B129" s="3">
+        <v>2</v>
+      </c>
+      <c r="C129" t="s">
+        <v>100</v>
+      </c>
+      <c r="D129" t="s">
+        <v>15</v>
+      </c>
+      <c r="E129" t="s">
+        <v>15</v>
+      </c>
+      <c r="F129" t="s">
+        <v>11</v>
+      </c>
+      <c r="G129" t="s">
+        <v>15</v>
+      </c>
+      <c r="H129" t="s">
+        <v>46</v>
+      </c>
+      <c r="I129" t="s">
+        <v>11</v>
+      </c>
+      <c r="J129" t="s">
+        <v>26</v>
+      </c>
+      <c r="K129" t="s">
+        <v>11</v>
+      </c>
+      <c r="L129" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A130" s="3">
+        <v>128</v>
+      </c>
+      <c r="B130" s="3">
+        <v>2</v>
+      </c>
+      <c r="C130" t="s">
+        <v>163</v>
+      </c>
+      <c r="D130" t="s">
+        <v>15</v>
+      </c>
+      <c r="E130" t="s">
+        <v>15</v>
+      </c>
+      <c r="F130" t="s">
+        <v>11</v>
+      </c>
+      <c r="G130" t="s">
+        <v>15</v>
+      </c>
+      <c r="H130" t="s">
+        <v>164</v>
+      </c>
+      <c r="I130" t="s">
+        <v>11</v>
+      </c>
+      <c r="J130" t="s">
+        <v>167</v>
+      </c>
+      <c r="K130" t="s">
+        <v>11</v>
+      </c>
+      <c r="L130" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A131" s="3">
+        <v>129</v>
+      </c>
+      <c r="B131" s="3">
+        <v>2</v>
+      </c>
+      <c r="C131" t="s">
+        <v>100</v>
+      </c>
+      <c r="D131" t="s">
+        <v>15</v>
+      </c>
+      <c r="E131" t="s">
+        <v>15</v>
+      </c>
+      <c r="F131" t="s">
+        <v>11</v>
+      </c>
+      <c r="G131" t="s">
+        <v>15</v>
+      </c>
+      <c r="H131" t="s">
+        <v>270</v>
+      </c>
+      <c r="I131" t="s">
+        <v>11</v>
+      </c>
+      <c r="J131" t="s">
+        <v>37</v>
+      </c>
+      <c r="K131" t="s">
+        <v>11</v>
+      </c>
+      <c r="L131" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A132" s="3">
+        <v>130</v>
+      </c>
+      <c r="B132" s="3">
+        <v>2</v>
+      </c>
+      <c r="C132" t="s">
+        <v>123</v>
+      </c>
+      <c r="D132" t="s">
+        <v>11</v>
+      </c>
+      <c r="E132" t="s">
+        <v>11</v>
+      </c>
+      <c r="F132" t="s">
+        <v>11</v>
+      </c>
+      <c r="G132" t="s">
+        <v>15</v>
+      </c>
+      <c r="H132" t="s">
+        <v>137</v>
+      </c>
+      <c r="I132" t="s">
+        <v>11</v>
+      </c>
+      <c r="J132" t="s">
+        <v>167</v>
+      </c>
+      <c r="K132" t="s">
+        <v>11</v>
+      </c>
+      <c r="L132" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A133" s="3">
+        <v>131</v>
+      </c>
+      <c r="B133" s="3">
+        <v>3</v>
+      </c>
+      <c r="C133" t="s">
+        <v>123</v>
+      </c>
+      <c r="D133" t="s">
+        <v>11</v>
+      </c>
+      <c r="E133" t="s">
+        <v>11</v>
+      </c>
+      <c r="F133" t="s">
+        <v>11</v>
+      </c>
+      <c r="G133" t="s">
+        <v>15</v>
+      </c>
+      <c r="H133" t="s">
+        <v>271</v>
+      </c>
+      <c r="I133" t="s">
+        <v>11</v>
+      </c>
+      <c r="J133" t="s">
+        <v>170</v>
+      </c>
+      <c r="K133" t="s">
+        <v>11</v>
+      </c>
+      <c r="L133" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A134" s="3">
+        <v>132</v>
+      </c>
+      <c r="B134" s="3">
+        <v>2</v>
+      </c>
+      <c r="C134" t="s">
+        <v>123</v>
+      </c>
+      <c r="D134" t="s">
+        <v>11</v>
+      </c>
+      <c r="E134" t="s">
+        <v>11</v>
+      </c>
+      <c r="F134" t="s">
+        <v>11</v>
+      </c>
+      <c r="G134" t="s">
+        <v>15</v>
+      </c>
+      <c r="H134" t="s">
+        <v>46</v>
+      </c>
+      <c r="I134" t="s">
+        <v>11</v>
+      </c>
+      <c r="J134" t="s">
+        <v>170</v>
+      </c>
+      <c r="K134" t="s">
+        <v>11</v>
+      </c>
+      <c r="L134" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A135" s="3">
+        <v>133</v>
+      </c>
+      <c r="B135" s="3">
+        <v>3</v>
+      </c>
+      <c r="C135" t="s">
+        <v>100</v>
+      </c>
+      <c r="D135" t="s">
+        <v>15</v>
+      </c>
+      <c r="E135" t="s">
+        <v>15</v>
+      </c>
+      <c r="F135" t="s">
+        <v>11</v>
+      </c>
+      <c r="G135" t="s">
+        <v>15</v>
+      </c>
+      <c r="H135" t="s">
+        <v>246</v>
+      </c>
+      <c r="I135" t="s">
+        <v>11</v>
+      </c>
+      <c r="J135" t="s">
+        <v>170</v>
+      </c>
+      <c r="K135" t="s">
+        <v>11</v>
+      </c>
+      <c r="L135" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A136" s="3">
+        <v>134</v>
+      </c>
+      <c r="B136" s="3">
+        <v>2</v>
+      </c>
+      <c r="C136" t="s">
+        <v>240</v>
+      </c>
+      <c r="D136" t="s">
+        <v>15</v>
+      </c>
+      <c r="E136" t="s">
+        <v>15</v>
+      </c>
+      <c r="F136" t="s">
+        <v>11</v>
+      </c>
+      <c r="G136" t="s">
+        <v>15</v>
+      </c>
+      <c r="H136" t="s">
+        <v>46</v>
+      </c>
+      <c r="I136" t="s">
+        <v>11</v>
+      </c>
+      <c r="J136" t="s">
+        <v>167</v>
+      </c>
+      <c r="K136" t="s">
+        <v>11</v>
+      </c>
+      <c r="L136" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A137" s="3">
+        <v>135</v>
+      </c>
+      <c r="B137" s="3">
+        <v>3</v>
+      </c>
+      <c r="C137" t="s">
+        <v>240</v>
+      </c>
+      <c r="D137" t="s">
+        <v>15</v>
+      </c>
+      <c r="E137" t="s">
+        <v>15</v>
+      </c>
+      <c r="F137" t="s">
+        <v>11</v>
+      </c>
+      <c r="G137" t="s">
+        <v>15</v>
+      </c>
+      <c r="H137" t="s">
+        <v>271</v>
+      </c>
+      <c r="I137" t="s">
+        <v>11</v>
+      </c>
+      <c r="J137" t="s">
+        <v>170</v>
+      </c>
+      <c r="K137" t="s">
+        <v>11</v>
+      </c>
+      <c r="L137" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A138" s="3">
+        <v>136</v>
+      </c>
+      <c r="B138" s="3">
+        <v>5</v>
+      </c>
+      <c r="C138" t="s">
+        <v>274</v>
+      </c>
+      <c r="D138" t="s">
+        <v>15</v>
+      </c>
+      <c r="E138" t="s">
+        <v>15</v>
+      </c>
+      <c r="F138" t="s">
+        <v>15</v>
+      </c>
+      <c r="G138" t="s">
+        <v>15</v>
+      </c>
+      <c r="H138" t="s">
+        <v>275</v>
+      </c>
+      <c r="I138" t="s">
+        <v>11</v>
+      </c>
+      <c r="J138" t="s">
+        <v>37</v>
+      </c>
+      <c r="K138" t="s">
+        <v>11</v>
+      </c>
+      <c r="L138" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A139" s="3">
+        <v>137</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C139" t="s">
+        <v>10</v>
+      </c>
+      <c r="D139" t="s">
+        <v>11</v>
+      </c>
+      <c r="E139" t="s">
+        <v>11</v>
+      </c>
+      <c r="F139" t="s">
+        <v>11</v>
+      </c>
+      <c r="G139" t="s">
+        <v>11</v>
+      </c>
+      <c r="H139" t="s">
+        <v>10</v>
+      </c>
+      <c r="I139" t="s">
+        <v>11</v>
+      </c>
+      <c r="J139" t="s">
+        <v>230</v>
+      </c>
+      <c r="K139" t="s">
+        <v>11</v>
+      </c>
+      <c r="L139" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A140" s="3">
+        <v>138</v>
+      </c>
+      <c r="B140" s="3">
+        <v>3</v>
+      </c>
+      <c r="C140" t="s">
+        <v>264</v>
+      </c>
+      <c r="D140" t="s">
+        <v>15</v>
+      </c>
+      <c r="E140" t="s">
+        <v>15</v>
+      </c>
+      <c r="F140" t="s">
+        <v>11</v>
+      </c>
+      <c r="G140" t="s">
+        <v>15</v>
+      </c>
+      <c r="H140" t="s">
+        <v>46</v>
+      </c>
+      <c r="I140" t="s">
+        <v>11</v>
+      </c>
+      <c r="J140" t="s">
+        <v>43</v>
+      </c>
+      <c r="K140" t="s">
+        <v>11</v>
+      </c>
+      <c r="L140" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A141" s="3">
+        <v>139</v>
+      </c>
+      <c r="B141" s="3">
+        <v>2</v>
+      </c>
+      <c r="C141" t="s">
+        <v>279</v>
+      </c>
+      <c r="D141" t="s">
+        <v>15</v>
+      </c>
+      <c r="E141" t="s">
+        <v>15</v>
+      </c>
+      <c r="F141" t="s">
+        <v>11</v>
+      </c>
+      <c r="G141" t="s">
+        <v>15</v>
+      </c>
+      <c r="H141" t="s">
+        <v>46</v>
+      </c>
+      <c r="I141" t="s">
+        <v>11</v>
+      </c>
+      <c r="J141" t="s">
+        <v>230</v>
+      </c>
+      <c r="K141" t="s">
+        <v>11</v>
+      </c>
+      <c r="L141" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A142" s="3">
+        <v>140</v>
+      </c>
+      <c r="B142" s="3">
+        <v>1</v>
+      </c>
+      <c r="C142" t="s">
+        <v>281</v>
+      </c>
+      <c r="D142" t="s">
+        <v>15</v>
+      </c>
+      <c r="E142" t="s">
+        <v>15</v>
+      </c>
+      <c r="F142" t="s">
+        <v>11</v>
+      </c>
+      <c r="G142" t="s">
+        <v>15</v>
+      </c>
+      <c r="H142" t="s">
+        <v>249</v>
+      </c>
+      <c r="I142" t="s">
+        <v>11</v>
+      </c>
+      <c r="J142" t="s">
+        <v>26</v>
+      </c>
+      <c r="K142" t="s">
+        <v>11</v>
+      </c>
+      <c r="L142" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A143" s="3">
+        <v>141</v>
+      </c>
+      <c r="B143" s="3">
+        <v>2</v>
+      </c>
+      <c r="C143" t="s">
+        <v>264</v>
+      </c>
+      <c r="D143" t="s">
+        <v>15</v>
+      </c>
+      <c r="E143" t="s">
+        <v>15</v>
+      </c>
+      <c r="F143" t="s">
+        <v>11</v>
+      </c>
+      <c r="G143" t="s">
+        <v>15</v>
+      </c>
+      <c r="H143" t="s">
+        <v>46</v>
+      </c>
+      <c r="I143" t="s">
+        <v>11</v>
+      </c>
+      <c r="J143" t="s">
+        <v>37</v>
+      </c>
+      <c r="K143" t="s">
+        <v>11</v>
+      </c>
+      <c r="L143" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A144" s="3">
+        <v>142</v>
+      </c>
+      <c r="B144" s="3">
+        <v>2</v>
+      </c>
+      <c r="C144" t="s">
+        <v>240</v>
+      </c>
+      <c r="D144" t="s">
+        <v>15</v>
+      </c>
+      <c r="E144" t="s">
+        <v>15</v>
+      </c>
+      <c r="F144" t="s">
+        <v>11</v>
+      </c>
+      <c r="G144" t="s">
+        <v>15</v>
+      </c>
+      <c r="H144" t="s">
+        <v>46</v>
+      </c>
+      <c r="I144" t="s">
+        <v>11</v>
+      </c>
+      <c r="J144" t="s">
+        <v>284</v>
+      </c>
+      <c r="K144" t="s">
+        <v>11</v>
+      </c>
+      <c r="L144" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A145" s="3">
+        <v>143</v>
+      </c>
+      <c r="B145" s="3">
+        <v>1</v>
+      </c>
+      <c r="C145" t="s">
+        <v>288</v>
+      </c>
+      <c r="D145" t="s">
+        <v>11</v>
+      </c>
+      <c r="E145" t="s">
+        <v>11</v>
+      </c>
+      <c r="F145" t="s">
+        <v>11</v>
+      </c>
+      <c r="G145" t="s">
+        <v>15</v>
+      </c>
+      <c r="H145" t="s">
+        <v>173</v>
+      </c>
+      <c r="I145" t="s">
+        <v>11</v>
+      </c>
+      <c r="J145" t="s">
+        <v>37</v>
+      </c>
+      <c r="K145" t="s">
+        <v>11</v>
+      </c>
+      <c r="L145" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A146" s="3">
+        <v>144</v>
+      </c>
+      <c r="B146" s="3">
+        <v>1</v>
+      </c>
+      <c r="C146" t="s">
+        <v>286</v>
+      </c>
+      <c r="D146" t="s">
+        <v>15</v>
+      </c>
+      <c r="E146" t="s">
+        <v>15</v>
+      </c>
+      <c r="F146" t="s">
+        <v>11</v>
+      </c>
+      <c r="G146" t="s">
+        <v>15</v>
+      </c>
+      <c r="H146" t="s">
+        <v>106</v>
+      </c>
+      <c r="I146" t="s">
+        <v>11</v>
+      </c>
+      <c r="J146" t="s">
+        <v>43</v>
+      </c>
+      <c r="K146" t="s">
+        <v>15</v>
+      </c>
+      <c r="L146" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A147" s="3">
+        <v>145</v>
+      </c>
+      <c r="B147" s="3">
+        <v>2</v>
+      </c>
+      <c r="C147" t="s">
+        <v>123</v>
+      </c>
+      <c r="D147" t="s">
+        <v>15</v>
+      </c>
+      <c r="E147" t="s">
+        <v>15</v>
+      </c>
+      <c r="F147" t="s">
+        <v>11</v>
+      </c>
+      <c r="G147" t="s">
+        <v>15</v>
+      </c>
+      <c r="H147" t="s">
+        <v>146</v>
+      </c>
+      <c r="I147" t="s">
+        <v>11</v>
+      </c>
+      <c r="J147" t="s">
+        <v>37</v>
+      </c>
+      <c r="K147" t="s">
+        <v>11</v>
+      </c>
+      <c r="L147" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A148" s="3">
+        <v>146</v>
+      </c>
+      <c r="B148" s="3">
+        <v>1</v>
+      </c>
+      <c r="C148" t="s">
+        <v>291</v>
+      </c>
+      <c r="D148" t="s">
+        <v>11</v>
+      </c>
+      <c r="E148" t="s">
+        <v>15</v>
+      </c>
+      <c r="F148" t="s">
+        <v>11</v>
+      </c>
+      <c r="G148" t="s">
+        <v>15</v>
+      </c>
+      <c r="H148" t="s">
+        <v>292</v>
+      </c>
+      <c r="I148" t="s">
+        <v>11</v>
+      </c>
+      <c r="J148" t="s">
+        <v>37</v>
+      </c>
+      <c r="K148" t="s">
+        <v>11</v>
+      </c>
+      <c r="L148" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A149" s="3">
+        <v>147</v>
+      </c>
+      <c r="B149" s="3">
+        <v>6</v>
+      </c>
+      <c r="C149" t="s">
+        <v>105</v>
+      </c>
+      <c r="D149" t="s">
+        <v>15</v>
+      </c>
+      <c r="E149" t="s">
+        <v>15</v>
+      </c>
+      <c r="F149" t="s">
+        <v>15</v>
+      </c>
+      <c r="G149" t="s">
+        <v>15</v>
+      </c>
+      <c r="H149" t="s">
+        <v>294</v>
+      </c>
+      <c r="I149" t="s">
+        <v>11</v>
+      </c>
+      <c r="J149" t="s">
+        <v>43</v>
+      </c>
+      <c r="K149" t="s">
+        <v>11</v>
+      </c>
+      <c r="L149" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A150" s="3">
+        <v>148</v>
+      </c>
+      <c r="B150" s="3">
+        <v>2</v>
+      </c>
+      <c r="C150" t="s">
+        <v>240</v>
+      </c>
+      <c r="D150" t="s">
+        <v>15</v>
+      </c>
+      <c r="E150" t="s">
+        <v>15</v>
+      </c>
+      <c r="F150" t="s">
+        <v>11</v>
+      </c>
+      <c r="G150" t="s">
+        <v>15</v>
+      </c>
+      <c r="H150" t="s">
+        <v>46</v>
+      </c>
+      <c r="I150" t="s">
+        <v>11</v>
+      </c>
+      <c r="J150" t="s">
+        <v>37</v>
+      </c>
+      <c r="K150" t="s">
+        <v>11</v>
+      </c>
+      <c r="L150" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A151" s="3">
+        <v>149</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C151" t="s">
+        <v>128</v>
+      </c>
+      <c r="D151" t="s">
+        <v>15</v>
+      </c>
+      <c r="E151" t="s">
+        <v>15</v>
+      </c>
+      <c r="F151" t="s">
+        <v>15</v>
+      </c>
+      <c r="G151" t="s">
+        <v>15</v>
+      </c>
+      <c r="H151" t="s">
+        <v>297</v>
+      </c>
+      <c r="I151" t="s">
+        <v>11</v>
+      </c>
+      <c r="J151" t="s">
+        <v>167</v>
+      </c>
+      <c r="K151" t="s">
+        <v>11</v>
+      </c>
+      <c r="L151" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A152" s="3">
+        <v>150</v>
+      </c>
+      <c r="B152" s="3">
+        <v>1</v>
+      </c>
+      <c r="C152" t="s">
+        <v>91</v>
+      </c>
+      <c r="D152" t="s">
+        <v>11</v>
+      </c>
+      <c r="E152" t="s">
+        <v>11</v>
+      </c>
+      <c r="F152" t="s">
+        <v>11</v>
+      </c>
+      <c r="G152" t="s">
+        <v>11</v>
+      </c>
+      <c r="H152" t="s">
+        <v>249</v>
+      </c>
+      <c r="I152" t="s">
+        <v>11</v>
+      </c>
+      <c r="J152" t="s">
+        <v>284</v>
+      </c>
+      <c r="K152" t="s">
+        <v>11</v>
+      </c>
+      <c r="L152" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A153" s="3">
+        <v>151</v>
+      </c>
+      <c r="B153" s="3">
+        <v>1</v>
+      </c>
+      <c r="C153" t="s">
+        <v>286</v>
+      </c>
+      <c r="D153" t="s">
+        <v>15</v>
+      </c>
+      <c r="E153" t="s">
+        <v>15</v>
+      </c>
+      <c r="F153" t="s">
+        <v>11</v>
+      </c>
+      <c r="G153" t="s">
+        <v>15</v>
+      </c>
+      <c r="H153" t="s">
+        <v>173</v>
+      </c>
+      <c r="I153" t="s">
+        <v>11</v>
+      </c>
+      <c r="J153" t="s">
+        <v>37</v>
+      </c>
+      <c r="K153" t="s">
+        <v>11</v>
+      </c>
+      <c r="L153" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A154" s="3">
+        <v>152</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C154" t="s">
+        <v>10</v>
+      </c>
+      <c r="D154" t="s">
+        <v>11</v>
+      </c>
+      <c r="E154" t="s">
+        <v>11</v>
+      </c>
+      <c r="F154" t="s">
+        <v>11</v>
+      </c>
+      <c r="G154" t="s">
+        <v>11</v>
+      </c>
+      <c r="H154" t="s">
+        <v>10</v>
+      </c>
+      <c r="I154" t="s">
+        <v>11</v>
+      </c>
+      <c r="J154" t="s">
+        <v>37</v>
+      </c>
+      <c r="K154" t="s">
+        <v>11</v>
+      </c>
+      <c r="L154" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A155" s="3">
+        <v>153</v>
+      </c>
+      <c r="B155" s="3">
+        <v>1</v>
+      </c>
+      <c r="C155" t="s">
+        <v>91</v>
+      </c>
+      <c r="D155" t="s">
+        <v>11</v>
+      </c>
+      <c r="E155" t="s">
+        <v>11</v>
+      </c>
+      <c r="F155" t="s">
+        <v>11</v>
+      </c>
+      <c r="G155" t="s">
+        <v>11</v>
+      </c>
+      <c r="H155" t="s">
+        <v>249</v>
+      </c>
+      <c r="I155" t="s">
+        <v>11</v>
+      </c>
+      <c r="J155" t="s">
+        <v>284</v>
+      </c>
+      <c r="K155" t="s">
+        <v>11</v>
+      </c>
+      <c r="L155" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A156" s="3">
+        <v>154</v>
+      </c>
+      <c r="B156" s="3">
+        <v>2</v>
+      </c>
+      <c r="C156" t="s">
+        <v>100</v>
+      </c>
+      <c r="D156" t="s">
+        <v>15</v>
+      </c>
+      <c r="E156" t="s">
+        <v>15</v>
+      </c>
+      <c r="F156" t="s">
+        <v>11</v>
+      </c>
+      <c r="G156" t="s">
+        <v>15</v>
+      </c>
+      <c r="H156" t="s">
+        <v>137</v>
+      </c>
+      <c r="I156" t="s">
+        <v>11</v>
+      </c>
+      <c r="J156" t="s">
+        <v>37</v>
+      </c>
+      <c r="K156" t="s">
+        <v>11</v>
+      </c>
+      <c r="L156" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A157" s="3">
+        <v>155</v>
+      </c>
+      <c r="B157" s="3">
+        <v>1</v>
+      </c>
+      <c r="C157" t="s">
+        <v>91</v>
+      </c>
+      <c r="D157" t="s">
+        <v>15</v>
+      </c>
+      <c r="E157" t="s">
+        <v>15</v>
+      </c>
+      <c r="F157" t="s">
+        <v>11</v>
+      </c>
+      <c r="G157" t="s">
+        <v>15</v>
+      </c>
+      <c r="H157" t="s">
+        <v>249</v>
+      </c>
+      <c r="I157" t="s">
+        <v>11</v>
+      </c>
+      <c r="J157" t="s">
+        <v>230</v>
+      </c>
+      <c r="K157" t="s">
+        <v>11</v>
+      </c>
+      <c r="L157" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A158" s="3">
+        <v>156</v>
+      </c>
+      <c r="B158" s="3">
+        <v>1</v>
+      </c>
+      <c r="C158" t="s">
+        <v>286</v>
+      </c>
+      <c r="D158" t="s">
+        <v>15</v>
+      </c>
+      <c r="E158" t="s">
+        <v>15</v>
+      </c>
+      <c r="F158" t="s">
+        <v>11</v>
+      </c>
+      <c r="G158" t="s">
+        <v>15</v>
+      </c>
+      <c r="H158" t="s">
+        <v>303</v>
+      </c>
+      <c r="I158" t="s">
+        <v>11</v>
+      </c>
+      <c r="J158" t="s">
+        <v>37</v>
+      </c>
+      <c r="K158" t="s">
+        <v>11</v>
+      </c>
+      <c r="L158" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A159" s="3">
+        <v>157</v>
+      </c>
+      <c r="B159" s="3">
+        <v>2</v>
+      </c>
+      <c r="C159" t="s">
+        <v>49</v>
+      </c>
+      <c r="D159" t="s">
+        <v>15</v>
+      </c>
+      <c r="E159" t="s">
+        <v>15</v>
+      </c>
+      <c r="F159" t="s">
+        <v>11</v>
+      </c>
+      <c r="G159" t="s">
+        <v>15</v>
+      </c>
+      <c r="H159" t="s">
+        <v>305</v>
+      </c>
+      <c r="I159" t="s">
+        <v>11</v>
+      </c>
+      <c r="J159" t="s">
+        <v>37</v>
+      </c>
+      <c r="K159" t="s">
+        <v>11</v>
+      </c>
+      <c r="L159" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A160" s="3">
+        <v>158</v>
+      </c>
+      <c r="B160" s="3">
+        <v>2</v>
+      </c>
+      <c r="C160" t="s">
+        <v>49</v>
+      </c>
+      <c r="D160" t="s">
+        <v>15</v>
+      </c>
+      <c r="E160" t="s">
+        <v>15</v>
+      </c>
+      <c r="F160" t="s">
+        <v>11</v>
+      </c>
+      <c r="G160" t="s">
+        <v>15</v>
+      </c>
+      <c r="H160" t="s">
+        <v>305</v>
+      </c>
+      <c r="I160" t="s">
+        <v>11</v>
+      </c>
+      <c r="J160" t="s">
+        <v>37</v>
+      </c>
+      <c r="K160" t="s">
+        <v>11</v>
+      </c>
+      <c r="L160" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A161" s="3">
+        <v>159</v>
+      </c>
+      <c r="B161" s="3">
+        <v>2</v>
+      </c>
+      <c r="C161" t="s">
+        <v>100</v>
+      </c>
+      <c r="D161" t="s">
+        <v>15</v>
+      </c>
+      <c r="E161" t="s">
+        <v>15</v>
+      </c>
+      <c r="F161" t="s">
+        <v>11</v>
+      </c>
+      <c r="G161" t="s">
+        <v>15</v>
+      </c>
+      <c r="H161" t="s">
+        <v>137</v>
+      </c>
+      <c r="I161" t="s">
+        <v>11</v>
+      </c>
+      <c r="J161" t="s">
+        <v>284</v>
+      </c>
+      <c r="K161" t="s">
+        <v>11</v>
+      </c>
+      <c r="L161" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A162" s="3">
+        <v>160</v>
+      </c>
+      <c r="B162" s="3">
+        <v>2</v>
+      </c>
+      <c r="C162" t="s">
+        <v>100</v>
+      </c>
+      <c r="D162" t="s">
+        <v>15</v>
+      </c>
+      <c r="E162" t="s">
+        <v>15</v>
+      </c>
+      <c r="F162" t="s">
+        <v>11</v>
+      </c>
+      <c r="G162" t="s">
+        <v>15</v>
+      </c>
+      <c r="H162" t="s">
+        <v>305</v>
+      </c>
+      <c r="I162" t="s">
+        <v>11</v>
+      </c>
+      <c r="J162" t="s">
+        <v>230</v>
+      </c>
+      <c r="K162" t="s">
+        <v>11</v>
+      </c>
+      <c r="L162" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A163" s="3">
+        <v>161</v>
+      </c>
+      <c r="B163" s="3">
+        <v>2</v>
+      </c>
+      <c r="C163" t="s">
+        <v>100</v>
+      </c>
+      <c r="D163" t="s">
+        <v>15</v>
+      </c>
+      <c r="E163" t="s">
+        <v>15</v>
+      </c>
+      <c r="F163" t="s">
+        <v>11</v>
+      </c>
+      <c r="G163" t="s">
+        <v>15</v>
+      </c>
+      <c r="H163" t="s">
+        <v>305</v>
+      </c>
+      <c r="I163" t="s">
+        <v>11</v>
+      </c>
+      <c r="J163" t="s">
+        <v>230</v>
+      </c>
+      <c r="K163" t="s">
+        <v>11</v>
+      </c>
+      <c r="L163" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A164" s="3">
+        <v>162</v>
+      </c>
+      <c r="B164" s="3">
+        <v>2</v>
+      </c>
+      <c r="C164" t="s">
+        <v>265</v>
+      </c>
+      <c r="D164" t="s">
+        <v>15</v>
+      </c>
+      <c r="E164" t="s">
+        <v>15</v>
+      </c>
+      <c r="F164" t="s">
+        <v>11</v>
+      </c>
+      <c r="G164" t="s">
+        <v>15</v>
+      </c>
+      <c r="H164" t="s">
+        <v>305</v>
+      </c>
+      <c r="I164" t="s">
+        <v>11</v>
+      </c>
+      <c r="J164" t="s">
+        <v>230</v>
+      </c>
+      <c r="K164" t="s">
+        <v>11</v>
+      </c>
+      <c r="L164" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A165" s="3">
+        <v>163</v>
+      </c>
+      <c r="B165" s="3">
+        <v>2</v>
+      </c>
+      <c r="C165" t="s">
+        <v>100</v>
+      </c>
+      <c r="D165" t="s">
+        <v>15</v>
+      </c>
+      <c r="E165" t="s">
+        <v>15</v>
+      </c>
+      <c r="F165" t="s">
+        <v>11</v>
+      </c>
+      <c r="G165" t="s">
+        <v>15</v>
+      </c>
+      <c r="H165" t="s">
+        <v>46</v>
+      </c>
+      <c r="I165" t="s">
+        <v>11</v>
+      </c>
+      <c r="J165" t="s">
+        <v>26</v>
+      </c>
+      <c r="K165" t="s">
+        <v>15</v>
+      </c>
+      <c r="L165" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A166" s="3">
+        <v>164</v>
+      </c>
+      <c r="B166" s="3">
+        <v>4</v>
+      </c>
+      <c r="C166" t="s">
+        <v>265</v>
+      </c>
+      <c r="D166" t="s">
+        <v>15</v>
+      </c>
+      <c r="E166" t="s">
+        <v>15</v>
+      </c>
+      <c r="F166" t="s">
+        <v>15</v>
+      </c>
+      <c r="G166" t="s">
+        <v>15</v>
+      </c>
+      <c r="H166" t="s">
+        <v>310</v>
+      </c>
+      <c r="I166" t="s">
+        <v>11</v>
+      </c>
+      <c r="J166" t="s">
+        <v>284</v>
+      </c>
+      <c r="K166" t="s">
+        <v>11</v>
+      </c>
+      <c r="L166" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A167" s="3">
+        <v>165</v>
+      </c>
+      <c r="B167" s="3">
+        <v>2</v>
+      </c>
+      <c r="C167" t="s">
+        <v>265</v>
+      </c>
+      <c r="D167" t="s">
+        <v>15</v>
+      </c>
+      <c r="E167" t="s">
+        <v>15</v>
+      </c>
+      <c r="F167" t="s">
+        <v>11</v>
+      </c>
+      <c r="G167" t="s">
+        <v>15</v>
+      </c>
+      <c r="H167" t="s">
+        <v>24</v>
+      </c>
+      <c r="I167" t="s">
+        <v>11</v>
+      </c>
+      <c r="J167" t="s">
+        <v>37</v>
+      </c>
+      <c r="K167" t="s">
+        <v>11</v>
+      </c>
+      <c r="L167" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A168" s="3">
+        <v>166</v>
+      </c>
+      <c r="B168" s="3">
+        <v>1</v>
+      </c>
+      <c r="C168" t="s">
+        <v>286</v>
+      </c>
+      <c r="D168" t="s">
+        <v>15</v>
+      </c>
+      <c r="E168" t="s">
+        <v>15</v>
+      </c>
+      <c r="F168" t="s">
+        <v>11</v>
+      </c>
+      <c r="G168" t="s">
+        <v>15</v>
+      </c>
+      <c r="H168" t="s">
+        <v>249</v>
+      </c>
+      <c r="I168" t="s">
+        <v>11</v>
+      </c>
+      <c r="J168" t="s">
+        <v>284</v>
+      </c>
+      <c r="K168" t="s">
+        <v>11</v>
+      </c>
+      <c r="L168" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A169" s="3">
+        <v>167</v>
+      </c>
+      <c r="B169" s="3">
+        <v>1</v>
+      </c>
+      <c r="C169" t="s">
+        <v>288</v>
+      </c>
+      <c r="D169" t="s">
+        <v>11</v>
+      </c>
+      <c r="E169" t="s">
+        <v>11</v>
+      </c>
+      <c r="F169" t="s">
+        <v>11</v>
+      </c>
+      <c r="G169" t="s">
+        <v>11</v>
+      </c>
+      <c r="H169" t="s">
+        <v>249</v>
+      </c>
+      <c r="I169" t="s">
+        <v>11</v>
+      </c>
+      <c r="J169" t="s">
+        <v>37</v>
+      </c>
+      <c r="K169" t="s">
+        <v>11</v>
+      </c>
+      <c r="L169" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A170" s="3">
+        <v>168</v>
+      </c>
+      <c r="B170" s="3">
+        <v>2</v>
+      </c>
+      <c r="C170" t="s">
+        <v>100</v>
+      </c>
+      <c r="D170" t="s">
+        <v>15</v>
+      </c>
+      <c r="E170" t="s">
+        <v>15</v>
+      </c>
+      <c r="F170" t="s">
+        <v>11</v>
+      </c>
+      <c r="G170" t="s">
+        <v>15</v>
+      </c>
+      <c r="H170" t="s">
+        <v>258</v>
+      </c>
+      <c r="I170" t="s">
+        <v>11</v>
+      </c>
+      <c r="J170" t="s">
+        <v>284</v>
+      </c>
+      <c r="K170" t="s">
+        <v>11</v>
+      </c>
+      <c r="L170" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A171" s="3">
+        <v>169</v>
+      </c>
+      <c r="B171" s="3">
+        <v>2</v>
+      </c>
+      <c r="C171" t="s">
+        <v>100</v>
+      </c>
+      <c r="D171" t="s">
+        <v>15</v>
+      </c>
+      <c r="E171" t="s">
+        <v>15</v>
+      </c>
+      <c r="F171" t="s">
+        <v>11</v>
+      </c>
+      <c r="G171" t="s">
+        <v>15</v>
+      </c>
+      <c r="H171" t="s">
+        <v>314</v>
+      </c>
+      <c r="I171" t="s">
+        <v>11</v>
+      </c>
+      <c r="J171" t="s">
+        <v>37</v>
+      </c>
+      <c r="K171" t="s">
+        <v>11</v>
+      </c>
+      <c r="L171" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A172" s="3">
+        <v>170</v>
+      </c>
+      <c r="B172" s="3">
+        <v>3</v>
+      </c>
+      <c r="C172" t="s">
+        <v>265</v>
+      </c>
+      <c r="D172" t="s">
+        <v>15</v>
+      </c>
+      <c r="E172" t="s">
+        <v>15</v>
+      </c>
+      <c r="F172" t="s">
+        <v>11</v>
+      </c>
+      <c r="G172" t="s">
+        <v>15</v>
+      </c>
+      <c r="H172" t="s">
+        <v>315</v>
+      </c>
+      <c r="I172" t="s">
+        <v>11</v>
+      </c>
+      <c r="J172" t="s">
+        <v>284</v>
+      </c>
+      <c r="K172" t="s">
+        <v>11</v>
+      </c>
+      <c r="L172" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A173" s="3">
+        <v>171</v>
+      </c>
+      <c r="B173" s="3">
+        <v>2</v>
+      </c>
+      <c r="C173" t="s">
+        <v>100</v>
+      </c>
+      <c r="D173" t="s">
+        <v>15</v>
+      </c>
+      <c r="E173" t="s">
+        <v>15</v>
+      </c>
+      <c r="F173" t="s">
+        <v>11</v>
+      </c>
+      <c r="G173" t="s">
+        <v>15</v>
+      </c>
+      <c r="H173" t="s">
+        <v>137</v>
+      </c>
+      <c r="I173" t="s">
+        <v>11</v>
+      </c>
+      <c r="J173" t="s">
+        <v>284</v>
+      </c>
+      <c r="K173" t="s">
+        <v>11</v>
+      </c>
+      <c r="L173" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A174" s="3">
+        <v>172</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C174" t="s">
+        <v>10</v>
+      </c>
+      <c r="D174" t="s">
+        <v>11</v>
+      </c>
+      <c r="E174" t="s">
+        <v>11</v>
+      </c>
+      <c r="F174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G174" t="s">
+        <v>11</v>
+      </c>
+      <c r="H174" t="s">
+        <v>10</v>
+      </c>
+      <c r="I174" t="s">
+        <v>11</v>
+      </c>
+      <c r="J174" t="s">
+        <v>37</v>
+      </c>
+      <c r="K174" t="s">
+        <v>11</v>
+      </c>
+      <c r="L174" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A175" s="3">
+        <v>173</v>
+      </c>
+      <c r="B175" s="3">
+        <v>2</v>
+      </c>
+      <c r="C175" t="s">
+        <v>100</v>
+      </c>
+      <c r="D175" t="s">
+        <v>15</v>
+      </c>
+      <c r="E175" t="s">
+        <v>15</v>
+      </c>
+      <c r="F175" t="s">
+        <v>11</v>
+      </c>
+      <c r="G175" t="s">
+        <v>15</v>
+      </c>
+      <c r="H175" t="s">
+        <v>152</v>
+      </c>
+      <c r="I175" t="s">
+        <v>11</v>
+      </c>
+      <c r="J175" t="s">
+        <v>37</v>
+      </c>
+      <c r="K175" t="s">
+        <v>11</v>
+      </c>
+      <c r="L175" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A176" s="3">
+        <v>174</v>
+      </c>
+      <c r="B176" s="3">
+        <v>2</v>
+      </c>
+      <c r="C176" t="s">
+        <v>100</v>
+      </c>
+      <c r="D176" t="s">
+        <v>15</v>
+      </c>
+      <c r="E176" t="s">
+        <v>15</v>
+      </c>
+      <c r="F176" t="s">
+        <v>11</v>
+      </c>
+      <c r="G176" t="s">
+        <v>15</v>
+      </c>
+      <c r="H176" t="s">
+        <v>46</v>
+      </c>
+      <c r="I176" t="s">
+        <v>11</v>
+      </c>
+      <c r="J176" t="s">
+        <v>284</v>
+      </c>
+      <c r="K176" t="s">
+        <v>11</v>
+      </c>
+      <c r="L176" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A177" s="3">
+        <v>175</v>
+      </c>
+      <c r="B177" s="3">
+        <v>2</v>
+      </c>
+      <c r="C177" t="s">
+        <v>240</v>
+      </c>
+      <c r="D177" t="s">
+        <v>15</v>
+      </c>
+      <c r="E177" t="s">
+        <v>15</v>
+      </c>
+      <c r="F177" t="s">
+        <v>11</v>
+      </c>
+      <c r="G177" t="s">
+        <v>15</v>
+      </c>
+      <c r="H177" t="s">
+        <v>46</v>
+      </c>
+      <c r="I177" t="s">
+        <v>11</v>
+      </c>
+      <c r="J177" t="s">
+        <v>284</v>
+      </c>
+      <c r="K177" t="s">
+        <v>11</v>
+      </c>
+      <c r="L177" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A178" s="3">
+        <v>176</v>
+      </c>
+      <c r="B178" s="3">
+        <v>2</v>
+      </c>
+      <c r="C178" t="s">
+        <v>100</v>
+      </c>
+      <c r="D178" t="s">
+        <v>15</v>
+      </c>
+      <c r="E178" t="s">
+        <v>15</v>
+      </c>
+      <c r="F178" t="s">
+        <v>11</v>
+      </c>
+      <c r="G178" t="s">
+        <v>15</v>
+      </c>
+      <c r="H178" t="s">
+        <v>46</v>
+      </c>
+      <c r="I178" t="s">
+        <v>11</v>
+      </c>
+      <c r="J178" t="s">
+        <v>37</v>
+      </c>
+      <c r="K178" t="s">
+        <v>11</v>
+      </c>
+      <c r="L178" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A179" s="3">
+        <v>177</v>
+      </c>
+      <c r="B179" s="3">
+        <v>2</v>
+      </c>
+      <c r="C179" t="s">
+        <v>100</v>
+      </c>
+      <c r="D179" t="s">
+        <v>15</v>
+      </c>
+      <c r="E179" t="s">
+        <v>15</v>
+      </c>
+      <c r="F179" t="s">
+        <v>11</v>
+      </c>
+      <c r="G179" t="s">
+        <v>15</v>
+      </c>
+      <c r="H179" t="s">
+        <v>24</v>
+      </c>
+      <c r="I179" t="s">
+        <v>11</v>
+      </c>
+      <c r="J179" t="s">
+        <v>37</v>
+      </c>
+      <c r="K179" t="s">
+        <v>11</v>
+      </c>
+      <c r="L179" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A180" s="3">
+        <v>178</v>
+      </c>
+      <c r="B180" s="3">
+        <v>2</v>
+      </c>
+      <c r="C180" t="s">
+        <v>123</v>
+      </c>
+      <c r="D180" t="s">
+        <v>15</v>
+      </c>
+      <c r="E180" t="s">
+        <v>15</v>
+      </c>
+      <c r="F180" t="s">
+        <v>11</v>
+      </c>
+      <c r="G180" t="s">
+        <v>15</v>
+      </c>
+      <c r="H180" t="s">
+        <v>46</v>
+      </c>
+      <c r="I180" t="s">
+        <v>11</v>
+      </c>
+      <c r="J180" t="s">
+        <v>37</v>
+      </c>
+      <c r="K180" t="s">
+        <v>11</v>
+      </c>
+      <c r="L180" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A181" s="3">
+        <v>179</v>
+      </c>
+      <c r="B181" s="3">
+        <v>2</v>
+      </c>
+      <c r="C181" t="s">
+        <v>100</v>
+      </c>
+      <c r="D181" t="s">
+        <v>15</v>
+      </c>
+      <c r="E181" t="s">
+        <v>15</v>
+      </c>
+      <c r="F181" t="s">
+        <v>11</v>
+      </c>
+      <c r="G181" t="s">
+        <v>15</v>
+      </c>
+      <c r="H181" t="s">
+        <v>46</v>
+      </c>
+      <c r="I181" t="s">
+        <v>11</v>
+      </c>
+      <c r="J181" t="s">
+        <v>284</v>
+      </c>
+      <c r="K181" t="s">
+        <v>11</v>
+      </c>
+      <c r="L181" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A182" s="3">
+        <v>180</v>
+      </c>
+      <c r="B182" s="3">
+        <v>2</v>
+      </c>
+      <c r="C182" t="s">
+        <v>240</v>
+      </c>
+      <c r="D182" t="s">
+        <v>15</v>
+      </c>
+      <c r="E182" t="s">
+        <v>15</v>
+      </c>
+      <c r="F182" t="s">
+        <v>11</v>
+      </c>
+      <c r="G182" t="s">
+        <v>15</v>
+      </c>
+      <c r="H182" t="s">
+        <v>61</v>
+      </c>
+      <c r="I182" t="s">
+        <v>11</v>
+      </c>
+      <c r="J182" t="s">
+        <v>37</v>
+      </c>
+      <c r="K182" t="s">
+        <v>11</v>
+      </c>
+      <c r="L182" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A183" s="3">
+        <v>181</v>
+      </c>
+      <c r="B183" s="3">
+        <v>2</v>
+      </c>
+      <c r="C183" t="s">
+        <v>240</v>
+      </c>
+      <c r="D183" t="s">
+        <v>15</v>
+      </c>
+      <c r="E183" t="s">
+        <v>15</v>
+      </c>
+      <c r="F183" t="s">
+        <v>11</v>
+      </c>
+      <c r="G183" t="s">
+        <v>15</v>
+      </c>
+      <c r="H183" t="s">
+        <v>61</v>
+      </c>
+      <c r="I183" t="s">
+        <v>11</v>
+      </c>
+      <c r="J183" t="s">
+        <v>284</v>
+      </c>
+      <c r="K183" t="s">
+        <v>11</v>
+      </c>
+      <c r="L183" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A184" s="3">
+        <v>182</v>
+      </c>
+      <c r="B184" s="3">
+        <v>2</v>
+      </c>
+      <c r="C184" t="s">
+        <v>100</v>
+      </c>
+      <c r="D184" t="s">
+        <v>15</v>
+      </c>
+      <c r="E184" t="s">
+        <v>15</v>
+      </c>
+      <c r="F184" t="s">
+        <v>11</v>
+      </c>
+      <c r="G184" t="s">
+        <v>15</v>
+      </c>
+      <c r="H184" t="s">
+        <v>137</v>
+      </c>
+      <c r="I184" t="s">
+        <v>11</v>
+      </c>
+      <c r="J184" t="s">
+        <v>284</v>
+      </c>
+      <c r="K184" t="s">
+        <v>15</v>
+      </c>
+      <c r="L184" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A185" s="3">
+        <v>183</v>
+      </c>
+      <c r="B185" s="3">
+        <v>1</v>
+      </c>
+      <c r="C185" t="s">
+        <v>286</v>
+      </c>
+      <c r="D185" t="s">
+        <v>15</v>
+      </c>
+      <c r="E185" t="s">
+        <v>15</v>
+      </c>
+      <c r="F185" t="s">
+        <v>15</v>
+      </c>
+      <c r="G185" t="s">
+        <v>15</v>
+      </c>
+      <c r="H185" t="s">
+        <v>249</v>
+      </c>
+      <c r="I185" t="s">
+        <v>11</v>
+      </c>
+      <c r="J185" t="s">
+        <v>37</v>
+      </c>
+      <c r="K185" t="s">
+        <v>11</v>
+      </c>
+      <c r="L185" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A186" s="3">
+        <v>184</v>
+      </c>
+      <c r="B186" s="3">
+        <v>2</v>
+      </c>
+      <c r="C186" t="s">
+        <v>240</v>
+      </c>
+      <c r="D186" t="s">
+        <v>15</v>
+      </c>
+      <c r="E186" t="s">
+        <v>15</v>
+      </c>
+      <c r="F186" t="s">
+        <v>11</v>
+      </c>
+      <c r="G186" t="s">
+        <v>15</v>
+      </c>
+      <c r="H186" t="s">
+        <v>323</v>
+      </c>
+      <c r="I186" t="s">
+        <v>11</v>
+      </c>
+      <c r="J186" t="s">
+        <v>37</v>
+      </c>
+      <c r="K186" t="s">
+        <v>11</v>
+      </c>
+      <c r="L186" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A187" s="3">
+        <v>185</v>
+      </c>
+      <c r="B187" s="3">
+        <v>2</v>
+      </c>
+      <c r="C187" t="s">
+        <v>128</v>
+      </c>
+      <c r="D187" t="s">
+        <v>15</v>
+      </c>
+      <c r="E187" t="s">
+        <v>15</v>
+      </c>
+      <c r="F187" t="s">
+        <v>15</v>
+      </c>
+      <c r="G187" t="s">
+        <v>15</v>
+      </c>
+      <c r="H187" t="s">
+        <v>314</v>
+      </c>
+      <c r="I187" t="s">
+        <v>11</v>
+      </c>
+      <c r="J187" t="s">
+        <v>284</v>
+      </c>
+      <c r="K187" t="s">
+        <v>11</v>
+      </c>
+      <c r="L187" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A188" s="3">
+        <v>186</v>
+      </c>
+      <c r="B188" s="3">
+        <v>2</v>
+      </c>
+      <c r="C188" t="s">
+        <v>265</v>
+      </c>
+      <c r="D188" t="s">
+        <v>15</v>
+      </c>
+      <c r="E188" t="s">
+        <v>15</v>
+      </c>
+      <c r="F188" t="s">
+        <v>11</v>
+      </c>
+      <c r="G188" t="s">
+        <v>15</v>
+      </c>
+      <c r="H188" t="s">
+        <v>325</v>
+      </c>
+      <c r="I188" t="s">
+        <v>11</v>
+      </c>
+      <c r="J188" t="s">
+        <v>284</v>
+      </c>
+      <c r="K188" t="s">
+        <v>11</v>
+      </c>
+      <c r="L188" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A189" s="3">
+        <v>187</v>
+      </c>
+      <c r="B189" s="3">
+        <v>2</v>
+      </c>
+      <c r="C189" t="s">
+        <v>100</v>
+      </c>
+      <c r="D189" t="s">
+        <v>15</v>
+      </c>
+      <c r="E189" t="s">
+        <v>15</v>
+      </c>
+      <c r="F189" t="s">
+        <v>15</v>
+      </c>
+      <c r="G189" t="s">
+        <v>15</v>
+      </c>
+      <c r="H189" t="s">
+        <v>46</v>
+      </c>
+      <c r="I189" t="s">
+        <v>11</v>
+      </c>
+      <c r="J189" t="s">
+        <v>284</v>
+      </c>
+      <c r="K189" t="s">
+        <v>11</v>
+      </c>
+      <c r="L189" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A190" s="3">
+        <v>188</v>
+      </c>
+      <c r="B190" s="3">
+        <v>1</v>
+      </c>
+      <c r="C190" t="s">
+        <v>91</v>
+      </c>
+      <c r="D190" t="s">
+        <v>11</v>
+      </c>
+      <c r="E190" t="s">
+        <v>11</v>
+      </c>
+      <c r="F190" t="s">
+        <v>11</v>
+      </c>
+      <c r="G190" t="s">
+        <v>15</v>
+      </c>
+      <c r="H190" t="s">
+        <v>249</v>
+      </c>
+      <c r="I190" t="s">
+        <v>11</v>
+      </c>
+      <c r="J190" t="s">
+        <v>284</v>
+      </c>
+      <c r="K190" t="s">
+        <v>11</v>
+      </c>
+      <c r="L190" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A191" s="3">
+        <v>189</v>
+      </c>
+      <c r="B191" s="3">
+        <v>2</v>
+      </c>
+      <c r="C191" t="s">
+        <v>100</v>
+      </c>
+      <c r="D191" t="s">
+        <v>15</v>
+      </c>
+      <c r="E191" t="s">
+        <v>15</v>
+      </c>
+      <c r="F191" t="s">
+        <v>11</v>
+      </c>
+      <c r="G191" t="s">
+        <v>15</v>
+      </c>
+      <c r="H191" t="s">
+        <v>141</v>
+      </c>
+      <c r="I191" t="s">
+        <v>11</v>
+      </c>
+      <c r="J191" t="s">
+        <v>284</v>
+      </c>
+      <c r="K191" t="s">
+        <v>15</v>
+      </c>
+      <c r="L191" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A192" s="3">
+        <v>190</v>
+      </c>
+      <c r="B192" s="3">
+        <v>1</v>
+      </c>
+      <c r="C192" t="s">
+        <v>327</v>
+      </c>
+      <c r="D192" t="s">
+        <v>11</v>
+      </c>
+      <c r="E192" t="s">
+        <v>11</v>
+      </c>
+      <c r="F192" t="s">
+        <v>11</v>
+      </c>
+      <c r="G192" t="s">
+        <v>15</v>
+      </c>
+      <c r="H192" t="s">
+        <v>173</v>
+      </c>
+      <c r="I192" t="s">
+        <v>11</v>
+      </c>
+      <c r="J192" t="s">
+        <v>37</v>
+      </c>
+      <c r="K192" t="s">
+        <v>11</v>
+      </c>
+      <c r="L192" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A193" s="3">
+        <v>191</v>
+      </c>
+      <c r="B193" s="3">
+        <v>3</v>
+      </c>
+      <c r="C193" t="s">
+        <v>100</v>
+      </c>
+      <c r="D193" t="s">
+        <v>15</v>
+      </c>
+      <c r="E193" t="s">
+        <v>15</v>
+      </c>
+      <c r="F193" t="s">
+        <v>11</v>
+      </c>
+      <c r="G193" t="s">
+        <v>15</v>
+      </c>
+      <c r="H193" t="s">
+        <v>329</v>
+      </c>
+      <c r="I193" t="s">
+        <v>11</v>
+      </c>
+      <c r="J193" t="s">
+        <v>37</v>
+      </c>
+      <c r="K193" t="s">
+        <v>11</v>
+      </c>
+      <c r="L193" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A194" s="3">
+        <v>192</v>
+      </c>
+      <c r="B194" s="3">
+        <v>2</v>
+      </c>
+      <c r="C194" t="s">
+        <v>265</v>
+      </c>
+      <c r="D194" t="s">
+        <v>15</v>
+      </c>
+      <c r="E194" t="s">
+        <v>15</v>
+      </c>
+      <c r="F194" t="s">
+        <v>11</v>
+      </c>
+      <c r="G194" t="s">
+        <v>15</v>
+      </c>
+      <c r="H194" t="s">
+        <v>46</v>
+      </c>
+      <c r="I194" t="s">
+        <v>11</v>
+      </c>
+      <c r="J194" t="s">
+        <v>284</v>
+      </c>
+      <c r="K194" t="s">
+        <v>11</v>
+      </c>
+      <c r="L194" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A195" s="3">
+        <v>193</v>
+      </c>
+      <c r="B195" s="3">
+        <v>2</v>
+      </c>
+      <c r="C195" t="s">
+        <v>286</v>
+      </c>
+      <c r="D195" t="s">
+        <v>15</v>
+      </c>
+      <c r="E195" t="s">
+        <v>15</v>
+      </c>
+      <c r="F195" t="s">
+        <v>11</v>
+      </c>
+      <c r="G195" t="s">
+        <v>15</v>
+      </c>
+      <c r="H195" t="s">
+        <v>331</v>
+      </c>
+      <c r="I195" t="s">
+        <v>11</v>
+      </c>
+      <c r="J195" t="s">
+        <v>37</v>
+      </c>
+      <c r="K195" t="s">
+        <v>11</v>
+      </c>
+      <c r="L195" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A196" s="3">
+        <v>194</v>
+      </c>
+      <c r="B196" s="3">
+        <v>2</v>
+      </c>
+      <c r="C196" t="s">
+        <v>265</v>
+      </c>
+      <c r="D196" t="s">
+        <v>11</v>
+      </c>
+      <c r="E196" t="s">
+        <v>11</v>
+      </c>
+      <c r="F196" t="s">
+        <v>11</v>
+      </c>
+      <c r="G196" t="s">
+        <v>15</v>
+      </c>
+      <c r="H196" t="s">
+        <v>333</v>
+      </c>
+      <c r="I196" t="s">
+        <v>11</v>
+      </c>
+      <c r="J196" t="s">
+        <v>37</v>
+      </c>
+      <c r="K196" t="s">
+        <v>11</v>
+      </c>
+      <c r="L196" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A197" s="3">
+        <v>195</v>
+      </c>
+      <c r="B197" s="3">
+        <v>2</v>
+      </c>
+      <c r="C197" t="s">
+        <v>49</v>
+      </c>
+      <c r="D197" t="s">
+        <v>15</v>
+      </c>
+      <c r="E197" t="s">
+        <v>15</v>
+      </c>
+      <c r="F197" t="s">
+        <v>11</v>
+      </c>
+      <c r="G197" t="s">
+        <v>15</v>
+      </c>
+      <c r="H197" t="s">
+        <v>335</v>
+      </c>
+      <c r="I197" t="s">
+        <v>11</v>
+      </c>
+      <c r="J197" t="s">
+        <v>37</v>
+      </c>
+      <c r="K197" t="s">
+        <v>11</v>
+      </c>
+      <c r="L197" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A198" s="3">
+        <v>196</v>
+      </c>
+      <c r="B198" s="3">
+        <v>2</v>
+      </c>
+      <c r="C198" t="s">
+        <v>100</v>
+      </c>
+      <c r="D198" t="s">
+        <v>15</v>
+      </c>
+      <c r="E198" t="s">
+        <v>15</v>
+      </c>
+      <c r="F198" t="s">
+        <v>11</v>
+      </c>
+      <c r="G198" t="s">
+        <v>15</v>
+      </c>
+      <c r="H198" t="s">
+        <v>336</v>
+      </c>
+      <c r="I198" t="s">
+        <v>11</v>
+      </c>
+      <c r="J198" t="s">
+        <v>167</v>
+      </c>
+      <c r="K198" t="s">
+        <v>11</v>
+      </c>
+      <c r="L198" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A199" s="3">
+        <v>197</v>
+      </c>
+      <c r="B199" s="3">
+        <v>2</v>
+      </c>
+      <c r="C199" t="s">
+        <v>123</v>
+      </c>
+      <c r="D199" t="s">
+        <v>11</v>
+      </c>
+      <c r="E199" t="s">
+        <v>11</v>
+      </c>
+      <c r="F199" t="s">
+        <v>11</v>
+      </c>
+      <c r="G199" t="s">
+        <v>11</v>
+      </c>
+      <c r="H199" t="s">
+        <v>333</v>
+      </c>
+      <c r="I199" t="s">
+        <v>11</v>
+      </c>
+      <c r="J199" t="s">
+        <v>37</v>
+      </c>
+      <c r="K199" t="s">
+        <v>11</v>
+      </c>
+      <c r="L199" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A200" s="3">
+        <v>198</v>
+      </c>
+      <c r="B200" s="3">
+        <v>2</v>
+      </c>
+      <c r="C200" t="s">
+        <v>49</v>
+      </c>
+      <c r="D200" t="s">
+        <v>15</v>
+      </c>
+      <c r="E200" t="s">
+        <v>15</v>
+      </c>
+      <c r="F200" t="s">
+        <v>11</v>
+      </c>
+      <c r="G200" t="s">
+        <v>15</v>
+      </c>
+      <c r="H200" t="s">
+        <v>338</v>
+      </c>
+      <c r="I200" t="s">
+        <v>11</v>
+      </c>
+      <c r="J200" t="s">
+        <v>37</v>
+      </c>
+      <c r="K200" t="s">
+        <v>11</v>
+      </c>
+      <c r="L200" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A201" s="3">
+        <v>199</v>
+      </c>
+      <c r="B201" s="3">
+        <v>2</v>
+      </c>
+      <c r="C201" t="s">
+        <v>100</v>
+      </c>
+      <c r="D201" t="s">
+        <v>15</v>
+      </c>
+      <c r="E201" t="s">
+        <v>15</v>
+      </c>
+      <c r="F201" t="s">
+        <v>11</v>
+      </c>
+      <c r="G201" t="s">
+        <v>15</v>
+      </c>
+      <c r="H201" t="s">
+        <v>141</v>
+      </c>
+      <c r="I201" t="s">
+        <v>11</v>
+      </c>
+      <c r="J201" t="s">
+        <v>37</v>
+      </c>
+      <c r="K201" t="s">
+        <v>11</v>
+      </c>
+      <c r="L201" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A202" s="3">
+        <v>200</v>
+      </c>
+      <c r="B202" s="3">
+        <v>2</v>
+      </c>
+      <c r="C202" t="s">
+        <v>49</v>
+      </c>
+      <c r="D202" t="s">
+        <v>15</v>
+      </c>
+      <c r="E202" t="s">
+        <v>15</v>
+      </c>
+      <c r="F202" t="s">
+        <v>11</v>
+      </c>
+      <c r="G202" t="s">
+        <v>15</v>
+      </c>
+      <c r="H202" t="s">
+        <v>141</v>
+      </c>
+      <c r="I202" t="s">
+        <v>11</v>
+      </c>
+      <c r="J202" t="s">
+        <v>37</v>
+      </c>
+      <c r="K202" t="s">
+        <v>11</v>
+      </c>
+      <c r="L202" t="s">
+        <v>257</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes up to Nov 25
</commit_message>
<xml_diff>
--- a/accident_ground_truths.xlsx
+++ b/accident_ground_truths.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryana\OneDrive\Documents\Actual Documents\extracted_frames_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8074D44E-5068-471D-9DE5-2AEE455E37B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D05105A-DDA8-4DF7-BC47-0AE6A1ED434F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="339">
   <si>
     <t>Number of vehicles in accident</t>
   </si>
@@ -1420,10 +1420,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L202"/>
+  <dimension ref="A1:L208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="B203" sqref="B203"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9107,6 +9107,234 @@
         <v>257</v>
       </c>
     </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A203" s="3">
+        <v>201</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C203" t="s">
+        <v>10</v>
+      </c>
+      <c r="D203" t="s">
+        <v>11</v>
+      </c>
+      <c r="E203" t="s">
+        <v>11</v>
+      </c>
+      <c r="F203" t="s">
+        <v>11</v>
+      </c>
+      <c r="G203" t="s">
+        <v>11</v>
+      </c>
+      <c r="H203" t="s">
+        <v>10</v>
+      </c>
+      <c r="I203" t="s">
+        <v>11</v>
+      </c>
+      <c r="J203" t="s">
+        <v>37</v>
+      </c>
+      <c r="K203" t="s">
+        <v>11</v>
+      </c>
+      <c r="L203" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A204" s="3">
+        <v>202</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C204" t="s">
+        <v>10</v>
+      </c>
+      <c r="D204" t="s">
+        <v>11</v>
+      </c>
+      <c r="E204" t="s">
+        <v>11</v>
+      </c>
+      <c r="F204" t="s">
+        <v>11</v>
+      </c>
+      <c r="G204" t="s">
+        <v>11</v>
+      </c>
+      <c r="H204" t="s">
+        <v>10</v>
+      </c>
+      <c r="I204" t="s">
+        <v>11</v>
+      </c>
+      <c r="J204" t="s">
+        <v>284</v>
+      </c>
+      <c r="K204" t="s">
+        <v>11</v>
+      </c>
+      <c r="L204" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A205" s="3">
+        <v>203</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C205" t="s">
+        <v>10</v>
+      </c>
+      <c r="D205" t="s">
+        <v>11</v>
+      </c>
+      <c r="E205" t="s">
+        <v>11</v>
+      </c>
+      <c r="F205" t="s">
+        <v>11</v>
+      </c>
+      <c r="G205" t="s">
+        <v>11</v>
+      </c>
+      <c r="H205" t="s">
+        <v>10</v>
+      </c>
+      <c r="I205" t="s">
+        <v>11</v>
+      </c>
+      <c r="J205" t="s">
+        <v>37</v>
+      </c>
+      <c r="K205" t="s">
+        <v>11</v>
+      </c>
+      <c r="L205" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A206" s="3">
+        <v>204</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C206" t="s">
+        <v>10</v>
+      </c>
+      <c r="D206" t="s">
+        <v>11</v>
+      </c>
+      <c r="E206" t="s">
+        <v>11</v>
+      </c>
+      <c r="F206" t="s">
+        <v>11</v>
+      </c>
+      <c r="G206" t="s">
+        <v>11</v>
+      </c>
+      <c r="H206" t="s">
+        <v>10</v>
+      </c>
+      <c r="I206" t="s">
+        <v>11</v>
+      </c>
+      <c r="J206" t="s">
+        <v>37</v>
+      </c>
+      <c r="K206" t="s">
+        <v>11</v>
+      </c>
+      <c r="L206" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A207" s="3">
+        <v>205</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C207" t="s">
+        <v>10</v>
+      </c>
+      <c r="D207" t="s">
+        <v>11</v>
+      </c>
+      <c r="E207" t="s">
+        <v>11</v>
+      </c>
+      <c r="F207" t="s">
+        <v>11</v>
+      </c>
+      <c r="G207" t="s">
+        <v>11</v>
+      </c>
+      <c r="H207" t="s">
+        <v>10</v>
+      </c>
+      <c r="I207" t="s">
+        <v>11</v>
+      </c>
+      <c r="J207" t="s">
+        <v>37</v>
+      </c>
+      <c r="K207" t="s">
+        <v>11</v>
+      </c>
+      <c r="L207" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A208" s="3">
+        <v>206</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C208" t="s">
+        <v>10</v>
+      </c>
+      <c r="D208" t="s">
+        <v>11</v>
+      </c>
+      <c r="E208" t="s">
+        <v>11</v>
+      </c>
+      <c r="F208" t="s">
+        <v>11</v>
+      </c>
+      <c r="G208" t="s">
+        <v>11</v>
+      </c>
+      <c r="H208" t="s">
+        <v>10</v>
+      </c>
+      <c r="I208" t="s">
+        <v>11</v>
+      </c>
+      <c r="J208" t="s">
+        <v>284</v>
+      </c>
+      <c r="K208" t="s">
+        <v>11</v>
+      </c>
+      <c r="L208" t="s">
+        <v>277</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>